<commit_message>
Backlog and Sprint 1 Updated
</commit_message>
<xml_diff>
--- a/Documentation/Product Backlog.xlsx
+++ b/Documentation/Product Backlog.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\congv\Documents\My_Studies\Fall-2019\COEN-390\COEN-390\Documentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F012C0-BC35-42CB-ADF1-85D21E5B4167}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19335" windowHeight="7560" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="5" r:id="rId1"/>
@@ -19,9 +13,10 @@
     <sheet name="Sprint 2" sheetId="3" r:id="rId4"/>
     <sheet name="Sprint 3" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="137">
   <si>
     <t>Story ID</t>
   </si>
@@ -94,9 +89,6 @@
     <t>Sprint 1</t>
   </si>
   <si>
-    <t>5 hrs</t>
-  </si>
-  <si>
     <t>FE-1</t>
   </si>
   <si>
@@ -133,9 +125,6 @@
     <t>GEN-2</t>
   </si>
   <si>
-    <t>As a presenter, I want to know when the sensor is not connected to the app so that I get to pair it with my phone (Story)</t>
-  </si>
-  <si>
     <t>BE-2</t>
   </si>
   <si>
@@ -148,10 +137,6 @@
     <t>The credit button will lead the presenter to another activity containing the information regarding the collaborators of the application</t>
   </si>
   <si>
-    <t>•Check if the sensor is connected to the phone
-•If the sensor is not connected, bring the user to the connection activity</t>
-  </si>
-  <si>
     <t>The Check Door button will allow the user to access a camera and see who is at the door</t>
   </si>
   <si>
@@ -176,16 +161,10 @@
     <t>•Display a list of all authorized users</t>
   </si>
   <si>
-    <t>As a presenter, check the history of the usage of the door. (Story)</t>
-  </si>
-  <si>
     <t>The application monitors and registers those who have unlocked the door, it display the information once the user clicks the History button</t>
   </si>
   <si>
     <t>•Display the list of user who used the door when History is clicked</t>
-  </si>
-  <si>
-    <t>As a presenter, I want the motion sensor  detect if anyone is at the door and send a notification delivered in history activity (Story)</t>
   </si>
   <si>
     <t>Check Door button</t>
@@ -195,9 +174,6 @@
 •Sensor is detecting movement and sending a notification to the application</t>
   </si>
   <si>
-    <t>The presenter wants to always know if the motion sensor is connected to the phone. If it is not connected, the application will bring the presenter to another activity that will allow him/her to connect to the sensor.</t>
-  </si>
-  <si>
     <t>As a presenter, I want the ability to see who is at the door when the motion sensor is activated  and notifies me using the first button. (Story)</t>
   </si>
   <si>
@@ -223,9 +199,6 @@
     <t>Unlock Door</t>
   </si>
   <si>
-    <t>Sensor Connected</t>
-  </si>
-  <si>
     <t>The motion sensor notifies me when someone is at the door by detecting something with the motion sensor.</t>
   </si>
   <si>
@@ -244,9 +217,6 @@
     <t>Main Page Button</t>
   </si>
   <si>
-    <t>1 hrs</t>
-  </si>
-  <si>
     <t>BE-4</t>
   </si>
   <si>
@@ -281,15 +251,6 @@
   </si>
   <si>
     <t xml:space="preserve"> F3-3</t>
-  </si>
-  <si>
-    <t>2 hrs</t>
-  </si>
-  <si>
-    <t>3 hrs</t>
-  </si>
-  <si>
-    <t>Sprint 1 Goal(s): Finish the project's skeleton</t>
   </si>
   <si>
     <t>There will be 5 buttons on the main page. The first one will allow the user to check the what is in front of the door, the second will be used to open a door, the third will be used to to show the user who has access to the door. The fourth used to see who last used the door and finally the last button shows the application credits</t>
@@ -310,12 +271,186 @@
   <si>
     <t>•Clicking button unlocks the door</t>
   </si>
+  <si>
+    <t>Learn Firebase</t>
+  </si>
+  <si>
+    <t>BE-5</t>
+  </si>
+  <si>
+    <t>As a presenter, I want to check the history of the usage of the door. (Story)</t>
+  </si>
+  <si>
+    <t>The application monitors and registers those who have unlocked the door, it display the pictures took once the user clicks the History button</t>
+  </si>
+  <si>
+    <t>Sprint 1 Goal(s): Finish the back-end, front-end of the project</t>
+  </si>
+  <si>
+    <t>There will be 5 buttons on the main page. The first one will allow the user to check the what is in front of the door, the second will be used to open a door, the third will be used to to show the user who has access to the door. The fourth used to see who last used the door and finally the last button shows the application credits. (See Documentation/Layout_Pictures/main_page)</t>
+  </si>
+  <si>
+    <t>Setup Database</t>
+  </si>
+  <si>
+    <t>As a user, I want my profile to be saved (Story)</t>
+  </si>
+  <si>
+    <t>The user's profile should be saved in a database, using Firebase.</t>
+  </si>
+  <si>
+    <t>•Able to add a profile to the database
+•Able to get the profile from the database</t>
+  </si>
+  <si>
+    <t>As a presenter, I want the motion sensor  detect if anyone is at the door and send a notification delivered in history activity (Epic)</t>
+  </si>
+  <si>
+    <t>BE-2.1</t>
+  </si>
+  <si>
+    <t>Connect Sensor to Arduino Board</t>
+  </si>
+  <si>
+    <t>The Arduino should be able to receive the data from the sensor.</t>
+  </si>
+  <si>
+    <t>BE-2.2</t>
+  </si>
+  <si>
+    <t>BE-2.3</t>
+  </si>
+  <si>
+    <t>Connect Arduino to Bluetooth</t>
+  </si>
+  <si>
+    <t>If the user creates a profile, check for valid name and password.</t>
+  </si>
+  <si>
+    <t>GEN-1.1</t>
+  </si>
+  <si>
+    <t>GEN-1.2</t>
+  </si>
+  <si>
+    <t>BE-3.1</t>
+  </si>
+  <si>
+    <t>BE-3.2</t>
+  </si>
+  <si>
+    <t>Learn how to use Firebase.</t>
+  </si>
+  <si>
+    <t>Motion Sensor</t>
+  </si>
+  <si>
+    <t>Learn the behaviour of the senors, inputs and outputs.</t>
+  </si>
+  <si>
+    <t>As a presenter, I want to know when the board is not connected to the app so that I get to pair it with my phone (Story)</t>
+  </si>
+  <si>
+    <t>Board Connected</t>
+  </si>
+  <si>
+    <t>•Check if the board is connected to the phone
+•If the sensor is not connected, bring the user to the connection activity</t>
+  </si>
+  <si>
+    <t>Connect Camera to Application</t>
+  </si>
+  <si>
+    <t>The camera should capture the view in front of the door if the motion sensor detects movement.</t>
+  </si>
+  <si>
+    <t>•Camera is connected
+•Camera takes a picture if sensor detects movement</t>
+  </si>
+  <si>
+    <t>Investigate how to use Aduino and use the I/O ports. Check the analog and digital I/O ports.</t>
+  </si>
+  <si>
+    <t>BE-4.1</t>
+  </si>
+  <si>
+    <t>BE-4.2</t>
+  </si>
+  <si>
+    <t>BE-4.3</t>
+  </si>
+  <si>
+    <t>BE-2.4</t>
+  </si>
+  <si>
+    <t>Learn Arduino for Sensor</t>
+  </si>
+  <si>
+    <t>hrs</t>
+  </si>
+  <si>
+    <t>Connect Camera to Arduino Board</t>
+  </si>
+  <si>
+    <t>The Arduino should be able to receive the data from the camera.</t>
+  </si>
+  <si>
+    <t>As a presenter, I want to be able to see who is at the door. (Story)</t>
+  </si>
+  <si>
+    <t>Total ideal Hours:</t>
+  </si>
+  <si>
+    <t>Storing Pictures in Database</t>
+  </si>
+  <si>
+    <t>Learn how to store pictures into a database.</t>
+  </si>
+  <si>
+    <t>BE-3.3</t>
+  </si>
+  <si>
+    <t>The presenter wants to always know if the board is connected to the phone. If it is not connected, the application will bring the presenter to another activity that will allow him/her to connect to the board.</t>
+  </si>
+  <si>
+    <t>BE-2.5</t>
+  </si>
+  <si>
+    <t>Coding Arduino Sensor</t>
+  </si>
+  <si>
+    <t>BE-2.6</t>
+  </si>
+  <si>
+    <t>Coding Bluetooth Sensor</t>
+  </si>
+  <si>
+    <t>Coding Arduino to send and receive signals from the sensor using thresholds.</t>
+  </si>
+  <si>
+    <t>Coding Bluetooth Camera</t>
+  </si>
+  <si>
+    <t>The Arduino should be able to communicate application using Bluetooth.</t>
+  </si>
+  <si>
+    <t>Coding Arduino Camera</t>
+  </si>
+  <si>
+    <t>Coding Arduino to send and receive signals from camera.</t>
+  </si>
+  <si>
+    <t>Coding Arduino to send camera pictures using Bluetooth.</t>
+  </si>
+  <si>
+    <t>Coding Arduino to send signals using Bluetooth.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,7 +569,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -488,6 +623,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -549,7 +687,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -584,7 +722,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -761,81 +899,81 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="126.6640625" customWidth="1"/>
+    <col min="1" max="1" width="126.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="7" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:1" s="7" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" s="7" customFormat="1" ht="13.5" customHeight="1"/>
+    <row r="2" spans="1:1" s="7" customFormat="1"/>
+    <row r="3" spans="1:1" s="7" customFormat="1" ht="26.25">
       <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" s="7" customFormat="1"/>
+    <row r="5" spans="1:1" s="7" customFormat="1"/>
+    <row r="6" spans="1:1" s="7" customFormat="1">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" s="7" customFormat="1">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:1" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:1" s="7" customFormat="1" ht="21">
       <c r="A8" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:1" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" s="7" customFormat="1"/>
+    <row r="10" spans="1:1" s="11" customFormat="1" ht="18.75">
       <c r="A10" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:1" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" s="11" customFormat="1" ht="18.75">
       <c r="A11" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:1" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" s="11" customFormat="1" ht="18.75">
       <c r="A12" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="17" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="18" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="19" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="20" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="21" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="22" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="23" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="24" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="25" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="26" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="27" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="28" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="29" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="30" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:1" s="7" customFormat="1"/>
+    <row r="14" spans="1:1" s="7" customFormat="1"/>
+    <row r="15" spans="1:1" s="7" customFormat="1"/>
+    <row r="16" spans="1:1" s="7" customFormat="1"/>
+    <row r="17" s="7" customFormat="1"/>
+    <row r="18" s="7" customFormat="1"/>
+    <row r="19" s="7" customFormat="1"/>
+    <row r="20" s="7" customFormat="1"/>
+    <row r="21" s="7" customFormat="1"/>
+    <row r="22" s="7" customFormat="1"/>
+    <row r="23" s="7" customFormat="1"/>
+    <row r="24" s="7" customFormat="1"/>
+    <row r="25" s="7" customFormat="1"/>
+    <row r="26" s="7" customFormat="1"/>
+    <row r="27" s="7" customFormat="1"/>
+    <row r="28" s="7" customFormat="1"/>
+    <row r="29" s="7" customFormat="1"/>
+    <row r="30" s="7" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -843,28 +981,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView topLeftCell="A14" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="44.44140625" customWidth="1"/>
-    <col min="4" max="4" width="7.44140625" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" customWidth="1"/>
-    <col min="7" max="7" width="43.109375" customWidth="1"/>
-    <col min="8" max="8" width="42.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="44.42578125" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="46.7109375" customWidth="1"/>
+    <col min="8" max="8" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="21">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -876,7 +1014,7 @@
       <c r="G1" s="20"/>
       <c r="H1" s="20"/>
     </row>
-    <row r="5" spans="1:8" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="17" customFormat="1" ht="40.5" customHeight="1">
       <c r="A5" s="16" t="s">
         <v>0</v>
       </c>
@@ -902,15 +1040,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="120">
       <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="C6" s="15" t="s">
         <v>23</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>24</v>
       </c>
       <c r="D6" s="3">
         <v>1</v>
@@ -922,13 +1060,13 @@
         <v>20</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="2"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -938,15 +1076,15 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="60">
       <c r="A8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>26</v>
-      </c>
       <c r="C8" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="3">
         <v>1</v>
@@ -958,13 +1096,13 @@
         <v>20</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="2"/>
       <c r="B9" s="14"/>
       <c r="C9" s="12"/>
@@ -974,33 +1112,33 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="30">
       <c r="A10" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="D10" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="2"/>
       <c r="B11" s="14"/>
       <c r="C11" s="12"/>
@@ -1010,54 +1148,44 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="45">
       <c r="A12" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B12" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="45">
+      <c r="A14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="2">
-        <v>3</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-    </row>
-    <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>45</v>
-      </c>
       <c r="D14" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>20</v>
@@ -1066,13 +1194,13 @@
         <v>20</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="2"/>
       <c r="B15" s="14"/>
       <c r="C15" s="12"/>
@@ -1082,18 +1210,18 @@
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
     </row>
-    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="60">
       <c r="A16" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="D16" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>20</v>
@@ -1102,13 +1230,13 @@
         <v>20</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="2"/>
       <c r="B17" s="14"/>
       <c r="C17" s="12"/>
@@ -1118,33 +1246,33 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
     </row>
-    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="45">
       <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="14" t="s">
-        <v>31</v>
-      </c>
       <c r="C18" s="12" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="D18" s="2">
         <v>2</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="2"/>
       <c r="B19" s="14"/>
       <c r="C19" s="12"/>
@@ -1154,33 +1282,33 @@
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
     </row>
-    <row r="20" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="76.5" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>34</v>
+        <v>105</v>
       </c>
       <c r="D20" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>54</v>
+        <v>125</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="24.75" customHeight="1">
       <c r="A21" s="2"/>
       <c r="B21" s="14"/>
       <c r="C21" s="12"/>
@@ -1190,33 +1318,33 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
     </row>
-    <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="30" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="D22" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="30" customHeight="1">
       <c r="A23" s="2"/>
       <c r="B23" s="14"/>
       <c r="C23" s="12"/>
@@ -1226,92 +1354,174 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
     </row>
-    <row r="24" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="30" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="B24" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="30" customHeight="1">
+      <c r="A25" s="2"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+    </row>
+    <row r="26" spans="1:8" ht="45">
+      <c r="A26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="2">
+        <v>3</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="2"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+    </row>
+    <row r="28" spans="1:8" ht="30">
+      <c r="A28" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="2">
+        <v>5</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" s="2">
+      <c r="F28" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="2"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+    </row>
+    <row r="30" spans="1:8" ht="45">
+      <c r="A30" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="2">
         <v>3</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B25" s="14" t="s">
+      <c r="E30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="2"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+    </row>
+    <row r="32" spans="1:8" ht="45">
+      <c r="A32" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" s="2">
-        <v>2</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G25" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="H25" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-    </row>
-    <row r="27" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D27" s="2">
+      <c r="B32" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="2">
         <v>3</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="H27" s="14" t="s">
-        <v>77</v>
+      <c r="E32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1319,22 +1529,22 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <dataValidations count="8">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Is the task completed?" prompt="Describe the criteria to be used to determine if the task is completed as per requirements._x000a_" sqref="H5" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task status" prompt="Current status of task. One of: Planned, In Progress, On Hold, Completed" sqref="F4 F38 F40:F1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task status" prompt="Current status of task. One of: Planned, In Progress, On Hold, Completed" sqref="F35:F1048576 F33 F4">
       <formula1>"Planned, In Progress, On Hold, Completed"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E5" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Card. One of: Planned, In Progress, On Hold, Completed" sqref="F5" xr:uid="{00000000-0002-0000-0100-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Story Point" prompt="Story point is an arbitary measure used to measure the effort required to implement a story._x000a__x000a_" sqref="D5" xr:uid="{00000000-0002-0000-0100-000004000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Priority" prompt="Priority of task. One of: Critical, High, Medium, Low" sqref="E38 E40:E1048576" xr:uid="{00000000-0002-0000-0100-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Priority" prompt="Priority of task. One of: Critical, High, Medium, Low" sqref="E33 E35:E1048576">
       <formula1>"Critical, High, Medium, Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Story. One of: Planned, In Progress, On Hold, Completed" sqref="F6:F27" xr:uid="{00000000-0002-0000-0100-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Story. One of: Planned, In Progress, On Hold, Completed" sqref="F6:F12 F14:F32">
       <formula1>"Not in sprint, Sprint 1, Sprint 2, Sprint 3, In Progress, On Hold, Completed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E6:E27" xr:uid="{00000000-0002-0000-0100-000007000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E6:E12 E14:E32">
       <formula1>"Sprint 1, Sprint 2, Sprint 3, Future"</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Is the task completed?" prompt="Describe the criteria to be used to determine if the task is completed as per requirements.&#10;" sqref="H5"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E5"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Card. One of: Planned, In Progress, On Hold, Completed" sqref="F5"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Story Point" prompt="Story point is an arbitary measure used to measure the effort required to implement a story.&#10;&#10;" sqref="D5"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="60" orientation="landscape" r:id="rId1"/>
@@ -1342,26 +1552,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="25.109375" customWidth="1"/>
-    <col min="4" max="4" width="44.44140625" customWidth="1"/>
-    <col min="5" max="5" width="7.44140625" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" customWidth="1"/>
-    <col min="7" max="7" width="43.109375" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="44.42578125" customWidth="1"/>
+    <col min="5" max="6" width="7.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="21">
       <c r="A1" s="19" t="s">
         <v>9</v>
       </c>
@@ -1371,18 +1581,30 @@
       <c r="E1" s="19"/>
       <c r="F1" s="19"/>
       <c r="G1" s="19"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="19"/>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
       <c r="D4" s="21"/>
       <c r="E4" s="21"/>
       <c r="F4" s="21"/>
-    </row>
-    <row r="6" spans="1:7" s="6" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="21"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" s="22"/>
+      <c r="C5">
+        <f>SUM(E7:E24)</f>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="6" customFormat="1" ht="40.5" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
@@ -1398,247 +1620,504 @@
       <c r="E6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="5"/>
+      <c r="G6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="135">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" ht="45">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" ht="30">
+      <c r="A9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="3">
+        <v>3</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" ht="60">
+      <c r="A10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="3">
+        <v>5</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" ht="30">
+      <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="3">
+        <v>3</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" ht="45">
+      <c r="A12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="3">
+        <v>5</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" ht="30">
+      <c r="A13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14" s="2">
+        <v>5</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" ht="30">
+      <c r="A15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="E15" s="2">
+        <v>5</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" ht="30">
+      <c r="A16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="D16" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="2">
+        <v>5</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" ht="30">
+      <c r="A17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="E17" s="2">
+        <v>5</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F10" s="3" t="s">
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" ht="30">
+      <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18" s="2">
+        <v>3</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" ht="30">
+      <c r="A19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" s="2">
+        <v>5</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F12" s="3" t="s">
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" ht="30">
+      <c r="A20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="E20" s="2">
+        <v>5</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="3" t="s">
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" ht="30">
+      <c r="A21" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="E21" s="2">
+        <v>5</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="E22" s="2">
+        <v>5</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" ht="75">
+      <c r="A23" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="E23" s="2">
+        <v>5</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" ht="30">
+      <c r="A24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E24" s="2">
+        <v>5</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" ht="30">
+      <c r="A25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="E25" s="2">
+        <v>5</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" ht="30">
+      <c r="A26" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E26" s="2">
+        <v>5</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H26" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A4:F4"/>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="F6" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimate" prompt="Estimated hours for the task." sqref="E6" xr:uid="{00000000-0002-0000-0200-000001000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="F7:F23" xr:uid="{00000000-0002-0000-0200-000002000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G6"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimate" prompt="Estimated hours for the task." sqref="E6:F6"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G7:G26">
       <formula1>"Planned, In Progress, On Hold, Completed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1648,14 +2127,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1663,12 +2142,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Minor Correction in Sprint 1
</commit_message>
<xml_diff>
--- a/Documentation/Product Backlog.xlsx
+++ b/Documentation/Product Backlog.xlsx
@@ -14,7 +14,6 @@
     <sheet name="Sprint 3" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -899,7 +898,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -987,7 +986,7 @@
   </sheetPr>
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+    <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -1210,7 +1209,7 @@
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
     </row>
-    <row r="16" spans="1:8" ht="60">
+    <row r="16" spans="1:8" ht="45">
       <c r="A16" s="2" t="s">
         <v>32</v>
       </c>
@@ -1558,8 +1557,8 @@
   </sheetPr>
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2062,7 +2061,7 @@
     </row>
     <row r="25" spans="1:8" ht="30">
       <c r="A25" s="2" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>113</v>

</xml_diff>

<commit_message>
Sprint 1 Assigned Tasks
</commit_message>
<xml_diff>
--- a/Documentation/Product Backlog.xlsx
+++ b/Documentation/Product Backlog.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\congv\Documents\My_Studies\Fall-2019\COEN-390\COEN-390\Documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD49468-D320-4EF0-8C41-8D90A9E36268}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19335" windowHeight="7560" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="5" r:id="rId1"/>
@@ -13,17 +19,23 @@
     <sheet name="Sprint 2" sheetId="3" r:id="rId4"/>
     <sheet name="Sprint 3" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="142">
   <si>
     <t>Story ID</t>
   </si>
@@ -444,12 +456,27 @@
   <si>
     <t>Coding Arduino to send signals using Bluetooth.</t>
   </si>
+  <si>
+    <t>Assigned to: Shadi Makdissi and Ogo-Oluwa Jesutomi Olasubulumi</t>
+  </si>
+  <si>
+    <t>Assigned to: Irfan Ahmed</t>
+  </si>
+  <si>
+    <t>Assigned to: Alec Kurkdjian and Cong-Vinh Vu</t>
+  </si>
+  <si>
+    <t>Assigned to: Alec Kurkdjian</t>
+  </si>
+  <si>
+    <t>Assigned to: Cong-Vinh Vu</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -898,81 +925,81 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="126.7109375" customWidth="1"/>
+    <col min="1" max="1" width="126.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="7" customFormat="1" ht="13.5" customHeight="1"/>
-    <row r="2" spans="1:1" s="7" customFormat="1"/>
-    <row r="3" spans="1:1" s="7" customFormat="1" ht="26.25">
+    <row r="1" spans="1:1" s="7" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:1" s="7" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="7" customFormat="1"/>
-    <row r="5" spans="1:1" s="7" customFormat="1"/>
-    <row r="6" spans="1:1" s="7" customFormat="1">
+    <row r="4" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="7" customFormat="1">
+    <row r="7" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:1" s="7" customFormat="1" ht="21">
+    <row r="8" spans="1:1" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A8" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" s="7" customFormat="1"/>
-    <row r="10" spans="1:1" s="11" customFormat="1" ht="18.75">
+    <row r="9" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:1" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:1" s="11" customFormat="1" ht="18.75">
+    <row r="11" spans="1:1" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:1" s="11" customFormat="1" ht="18.75">
+    <row r="12" spans="1:1" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:1" s="7" customFormat="1"/>
-    <row r="14" spans="1:1" s="7" customFormat="1"/>
-    <row r="15" spans="1:1" s="7" customFormat="1"/>
-    <row r="16" spans="1:1" s="7" customFormat="1"/>
-    <row r="17" s="7" customFormat="1"/>
-    <row r="18" s="7" customFormat="1"/>
-    <row r="19" s="7" customFormat="1"/>
-    <row r="20" s="7" customFormat="1"/>
-    <row r="21" s="7" customFormat="1"/>
-    <row r="22" s="7" customFormat="1"/>
-    <row r="23" s="7" customFormat="1"/>
-    <row r="24" s="7" customFormat="1"/>
-    <row r="25" s="7" customFormat="1"/>
-    <row r="26" s="7" customFormat="1"/>
-    <row r="27" s="7" customFormat="1"/>
-    <row r="28" s="7" customFormat="1"/>
-    <row r="29" s="7" customFormat="1"/>
-    <row r="30" s="7" customFormat="1"/>
+    <row r="13" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="17" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="18" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="19" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="21" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="22" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="23" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="24" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="25" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="26" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="27" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="28" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="29" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="30" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -980,7 +1007,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -990,18 +1017,18 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="44.42578125" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="46.7109375" customWidth="1"/>
-    <col min="8" max="8" width="42.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="44.44140625" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1"/>
+    <col min="7" max="7" width="46.6640625" customWidth="1"/>
+    <col min="8" max="8" width="42.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -1013,7 +1040,7 @@
       <c r="G1" s="20"/>
       <c r="H1" s="20"/>
     </row>
-    <row r="5" spans="1:8" s="17" customFormat="1" ht="40.5" customHeight="1">
+    <row r="5" spans="1:8" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>0</v>
       </c>
@@ -1039,7 +1066,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="120">
+    <row r="6" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
@@ -1065,7 +1092,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -1075,7 +1102,7 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="1:8" ht="60">
+    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
@@ -1101,7 +1128,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="14"/>
       <c r="C9" s="12"/>
@@ -1111,7 +1138,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:8" ht="30">
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>29</v>
       </c>
@@ -1137,7 +1164,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="14"/>
       <c r="C11" s="12"/>
@@ -1147,7 +1174,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:8" ht="45">
+    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -1173,7 +1200,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="45">
+    <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -1199,7 +1226,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="14"/>
       <c r="C15" s="12"/>
@@ -1209,7 +1236,7 @@
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
     </row>
-    <row r="16" spans="1:8" ht="45">
+    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>32</v>
       </c>
@@ -1235,7 +1262,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="14"/>
       <c r="C17" s="12"/>
@@ -1245,7 +1272,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
     </row>
-    <row r="18" spans="1:8" ht="45">
+    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
@@ -1271,7 +1298,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="14"/>
       <c r="C19" s="12"/>
@@ -1281,7 +1308,7 @@
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
     </row>
-    <row r="20" spans="1:8" ht="76.5" customHeight="1">
+    <row r="20" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>31</v>
       </c>
@@ -1307,7 +1334,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="24.75" customHeight="1">
+    <row r="21" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="14"/>
       <c r="C21" s="12"/>
@@ -1317,7 +1344,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
     </row>
-    <row r="22" spans="1:8" ht="30" customHeight="1">
+    <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
@@ -1343,7 +1370,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="30" customHeight="1">
+    <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="14"/>
       <c r="C23" s="12"/>
@@ -1353,7 +1380,7 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
     </row>
-    <row r="24" spans="1:8" ht="30" customHeight="1">
+    <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>63</v>
       </c>
@@ -1379,7 +1406,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="30" customHeight="1">
+    <row r="25" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="14"/>
       <c r="C25" s="12"/>
@@ -1389,7 +1416,7 @@
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
     </row>
-    <row r="26" spans="1:8" ht="45">
+    <row r="26" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>71</v>
       </c>
@@ -1415,7 +1442,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="14"/>
       <c r="C27" s="12"/>
@@ -1425,7 +1452,7 @@
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
     </row>
-    <row r="28" spans="1:8" ht="30">
+    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>63</v>
       </c>
@@ -1451,7 +1478,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="14"/>
       <c r="C29" s="12"/>
@@ -1461,7 +1488,7 @@
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
     </row>
-    <row r="30" spans="1:8" ht="45">
+    <row r="30" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>81</v>
       </c>
@@ -1487,7 +1514,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="14"/>
       <c r="C31" s="12"/>
@@ -1497,7 +1524,7 @@
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
     </row>
-    <row r="32" spans="1:8" ht="45">
+    <row r="32" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>72</v>
       </c>
@@ -1528,22 +1555,22 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task status" prompt="Current status of task. One of: Planned, In Progress, On Hold, Completed" sqref="F35:F1048576 F33 F4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task status" prompt="Current status of task. One of: Planned, In Progress, On Hold, Completed" sqref="F35:F1048576 F33 F4" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Planned, In Progress, On Hold, Completed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Priority" prompt="Priority of task. One of: Critical, High, Medium, Low" sqref="E33 E35:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Priority" prompt="Priority of task. One of: Critical, High, Medium, Low" sqref="E33 E35:E1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Critical, High, Medium, Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Story. One of: Planned, In Progress, On Hold, Completed" sqref="F6:F12 F14:F32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Story. One of: Planned, In Progress, On Hold, Completed" sqref="F6:F12 F14:F32" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Not in sprint, Sprint 1, Sprint 2, Sprint 3, In Progress, On Hold, Completed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E6:E12 E14:E32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E6:E12 E14:E32" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"Sprint 1, Sprint 2, Sprint 3, Future"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Is the task completed?" prompt="Describe the criteria to be used to determine if the task is completed as per requirements.&#10;" sqref="H5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Card. One of: Planned, In Progress, On Hold, Completed" sqref="F5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Story Point" prompt="Story point is an arbitary measure used to measure the effort required to implement a story.&#10;&#10;" sqref="D5"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Is the task completed?" prompt="Describe the criteria to be used to determine if the task is completed as per requirements._x000a_" sqref="H5" xr:uid="{00000000-0002-0000-0100-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E5" xr:uid="{00000000-0002-0000-0100-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Card. One of: Planned, In Progress, On Hold, Completed" sqref="F5" xr:uid="{00000000-0002-0000-0100-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Story Point" prompt="Story point is an arbitary measure used to measure the effort required to implement a story._x000a__x000a_" sqref="D5" xr:uid="{00000000-0002-0000-0100-000007000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="60" orientation="landscape" r:id="rId1"/>
@@ -1551,26 +1578,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="25.140625" customWidth="1"/>
-    <col min="4" max="4" width="44.42578125" customWidth="1"/>
-    <col min="5" max="6" width="7.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="43.140625" customWidth="1"/>
+    <col min="3" max="3" width="25.109375" customWidth="1"/>
+    <col min="4" max="4" width="44.44140625" customWidth="1"/>
+    <col min="5" max="6" width="7.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" customWidth="1"/>
+    <col min="8" max="8" width="43.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="19" t="s">
         <v>9</v>
       </c>
@@ -1582,7 +1609,7 @@
       <c r="G1" s="19"/>
       <c r="H1" s="19"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>84</v>
       </c>
@@ -1593,17 +1620,17 @@
       <c r="F4" s="21"/>
       <c r="G4" s="21"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>121</v>
       </c>
       <c r="B5" s="22"/>
       <c r="C5">
-        <f>SUM(E7:E24)</f>
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="6" customFormat="1" ht="40.5" customHeight="1">
+        <f>SUM(E7:E26)</f>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="6" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
@@ -1627,7 +1654,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="135">
+    <row r="7" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -1649,9 +1676,11 @@
       <c r="G7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" ht="45">
+      <c r="H7" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -1673,9 +1702,11 @@
       <c r="G8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" ht="30">
+      <c r="H8" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>73</v>
       </c>
@@ -1697,9 +1728,11 @@
       <c r="G9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" ht="60">
+      <c r="H9" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
@@ -1721,9 +1754,11 @@
       <c r="G10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" ht="30">
+      <c r="H10" s="14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
@@ -1745,9 +1780,11 @@
       <c r="G11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" ht="45">
+      <c r="H11" s="14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>28</v>
       </c>
@@ -1769,9 +1806,11 @@
       <c r="G12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" ht="30">
+      <c r="H12" s="13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>28</v>
       </c>
@@ -1793,9 +1832,11 @@
       <c r="G13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="H13" s="13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>34</v>
       </c>
@@ -1817,9 +1858,11 @@
       <c r="G14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" ht="30">
+      <c r="H14" s="14" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>34</v>
       </c>
@@ -1841,9 +1884,11 @@
       <c r="G15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" ht="30">
+      <c r="H15" s="14" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>34</v>
       </c>
@@ -1865,9 +1910,11 @@
       <c r="G16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" ht="30">
+      <c r="H16" s="14" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
@@ -1889,9 +1936,11 @@
       <c r="G17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" ht="30">
+      <c r="H17" s="14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
@@ -1913,9 +1962,11 @@
       <c r="G18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="1:8" ht="30">
+      <c r="H18" s="14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>33</v>
       </c>
@@ -1937,9 +1988,11 @@
       <c r="G19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:8" ht="30">
+      <c r="H19" s="14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>33</v>
       </c>
@@ -1961,9 +2014,11 @@
       <c r="G20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:8" ht="30">
+      <c r="H20" s="14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
@@ -1985,9 +2040,11 @@
       <c r="G21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="H21" s="14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>33</v>
       </c>
@@ -2009,9 +2066,11 @@
       <c r="G22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:8" ht="75">
+      <c r="H22" s="14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>31</v>
       </c>
@@ -2033,9 +2092,11 @@
       <c r="G23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:8" ht="30">
+      <c r="H23" s="14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>63</v>
       </c>
@@ -2057,9 +2118,11 @@
       <c r="G24" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:8" ht="30">
+      <c r="H24" s="14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>63</v>
       </c>
@@ -2081,9 +2144,11 @@
       <c r="G25" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:8" ht="30">
+      <c r="H25" s="14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>63</v>
       </c>
@@ -2105,7 +2170,9 @@
       <c r="G26" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H26" s="2"/>
+      <c r="H26" s="14" t="s">
+        <v>137</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2114,9 +2181,9 @@
     <mergeCell ref="A5:B5"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G6"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimate" prompt="Estimated hours for the task." sqref="E6:F6"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G7:G26">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G6" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimate" prompt="Estimated hours for the task." sqref="E6:F6" xr:uid="{00000000-0002-0000-0200-000001000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G7:G26" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>"Planned, In Progress, On Hold, Completed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2126,14 +2193,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2141,12 +2208,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Sprint 1 Cherry Pick
</commit_message>
<xml_diff>
--- a/Documentation/Product Backlog.xlsx
+++ b/Documentation/Product Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\congv\Documents\My_Studies\Fall-2019\COEN-390\COEN-390\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F012C0-BC35-42CB-ADF1-85D21E5B4167}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E2BD1A-8DF4-4F91-9C58-BACFBC01F6E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="5" r:id="rId1"/>
@@ -19,17 +19,23 @@
     <sheet name="Sprint 2" sheetId="3" r:id="rId4"/>
     <sheet name="Sprint 3" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="142">
   <si>
     <t>Story ID</t>
   </si>
@@ -94,9 +100,6 @@
     <t>Sprint 1</t>
   </si>
   <si>
-    <t>5 hrs</t>
-  </si>
-  <si>
     <t>FE-1</t>
   </si>
   <si>
@@ -133,9 +136,6 @@
     <t>GEN-2</t>
   </si>
   <si>
-    <t>As a presenter, I want to know when the sensor is not connected to the app so that I get to pair it with my phone (Story)</t>
-  </si>
-  <si>
     <t>BE-2</t>
   </si>
   <si>
@@ -148,10 +148,6 @@
     <t>The credit button will lead the presenter to another activity containing the information regarding the collaborators of the application</t>
   </si>
   <si>
-    <t>•Check if the sensor is connected to the phone
-•If the sensor is not connected, bring the user to the connection activity</t>
-  </si>
-  <si>
     <t>The Check Door button will allow the user to access a camera and see who is at the door</t>
   </si>
   <si>
@@ -176,16 +172,10 @@
     <t>•Display a list of all authorized users</t>
   </si>
   <si>
-    <t>As a presenter, check the history of the usage of the door. (Story)</t>
-  </si>
-  <si>
     <t>The application monitors and registers those who have unlocked the door, it display the information once the user clicks the History button</t>
   </si>
   <si>
     <t>•Display the list of user who used the door when History is clicked</t>
-  </si>
-  <si>
-    <t>As a presenter, I want the motion sensor  detect if anyone is at the door and send a notification delivered in history activity (Story)</t>
   </si>
   <si>
     <t>Check Door button</t>
@@ -195,9 +185,6 @@
 •Sensor is detecting movement and sending a notification to the application</t>
   </si>
   <si>
-    <t>The presenter wants to always know if the motion sensor is connected to the phone. If it is not connected, the application will bring the presenter to another activity that will allow him/her to connect to the sensor.</t>
-  </si>
-  <si>
     <t>As a presenter, I want the ability to see who is at the door when the motion sensor is activated  and notifies me using the first button. (Story)</t>
   </si>
   <si>
@@ -223,9 +210,6 @@
     <t>Unlock Door</t>
   </si>
   <si>
-    <t>Sensor Connected</t>
-  </si>
-  <si>
     <t>The motion sensor notifies me when someone is at the door by detecting something with the motion sensor.</t>
   </si>
   <si>
@@ -244,9 +228,6 @@
     <t>Main Page Button</t>
   </si>
   <si>
-    <t>1 hrs</t>
-  </si>
-  <si>
     <t>BE-4</t>
   </si>
   <si>
@@ -281,15 +262,6 @@
   </si>
   <si>
     <t xml:space="preserve"> F3-3</t>
-  </si>
-  <si>
-    <t>2 hrs</t>
-  </si>
-  <si>
-    <t>3 hrs</t>
-  </si>
-  <si>
-    <t>Sprint 1 Goal(s): Finish the project's skeleton</t>
   </si>
   <si>
     <t>There will be 5 buttons on the main page. The first one will allow the user to check the what is in front of the door, the second will be used to open a door, the third will be used to to show the user who has access to the door. The fourth used to see who last used the door and finally the last button shows the application credits</t>
@@ -309,6 +281,195 @@
   </si>
   <si>
     <t>•Clicking button unlocks the door</t>
+  </si>
+  <si>
+    <t>Learn Firebase</t>
+  </si>
+  <si>
+    <t>BE-5</t>
+  </si>
+  <si>
+    <t>As a presenter, I want to check the history of the usage of the door. (Story)</t>
+  </si>
+  <si>
+    <t>The application monitors and registers those who have unlocked the door, it display the pictures took once the user clicks the History button</t>
+  </si>
+  <si>
+    <t>Sprint 1 Goal(s): Finish the back-end, front-end of the project</t>
+  </si>
+  <si>
+    <t>There will be 5 buttons on the main page. The first one will allow the user to check the what is in front of the door, the second will be used to open a door, the third will be used to to show the user who has access to the door. The fourth used to see who last used the door and finally the last button shows the application credits. (See Documentation/Layout_Pictures/main_page)</t>
+  </si>
+  <si>
+    <t>Setup Database</t>
+  </si>
+  <si>
+    <t>As a user, I want my profile to be saved (Story)</t>
+  </si>
+  <si>
+    <t>The user's profile should be saved in a database, using Firebase.</t>
+  </si>
+  <si>
+    <t>•Able to add a profile to the database
+•Able to get the profile from the database</t>
+  </si>
+  <si>
+    <t>As a presenter, I want the motion sensor  detect if anyone is at the door and send a notification delivered in history activity (Epic)</t>
+  </si>
+  <si>
+    <t>BE-2.1</t>
+  </si>
+  <si>
+    <t>Connect Sensor to Arduino Board</t>
+  </si>
+  <si>
+    <t>The Arduino should be able to receive the data from the sensor.</t>
+  </si>
+  <si>
+    <t>BE-2.2</t>
+  </si>
+  <si>
+    <t>BE-2.3</t>
+  </si>
+  <si>
+    <t>Connect Arduino to Bluetooth</t>
+  </si>
+  <si>
+    <t>If the user creates a profile, check for valid name and password.</t>
+  </si>
+  <si>
+    <t>GEN-1.1</t>
+  </si>
+  <si>
+    <t>GEN-1.2</t>
+  </si>
+  <si>
+    <t>BE-3.1</t>
+  </si>
+  <si>
+    <t>BE-3.2</t>
+  </si>
+  <si>
+    <t>Learn how to use Firebase.</t>
+  </si>
+  <si>
+    <t>Motion Sensor</t>
+  </si>
+  <si>
+    <t>Learn the behaviour of the senors, inputs and outputs.</t>
+  </si>
+  <si>
+    <t>As a presenter, I want to know when the board is not connected to the app so that I get to pair it with my phone (Story)</t>
+  </si>
+  <si>
+    <t>Board Connected</t>
+  </si>
+  <si>
+    <t>•Check if the board is connected to the phone
+•If the sensor is not connected, bring the user to the connection activity</t>
+  </si>
+  <si>
+    <t>Connect Camera to Application</t>
+  </si>
+  <si>
+    <t>The camera should capture the view in front of the door if the motion sensor detects movement.</t>
+  </si>
+  <si>
+    <t>•Camera is connected
+•Camera takes a picture if sensor detects movement</t>
+  </si>
+  <si>
+    <t>Investigate how to use Aduino and use the I/O ports. Check the analog and digital I/O ports.</t>
+  </si>
+  <si>
+    <t>BE-4.1</t>
+  </si>
+  <si>
+    <t>BE-4.2</t>
+  </si>
+  <si>
+    <t>BE-4.3</t>
+  </si>
+  <si>
+    <t>BE-2.4</t>
+  </si>
+  <si>
+    <t>Learn Arduino for Sensor</t>
+  </si>
+  <si>
+    <t>hrs</t>
+  </si>
+  <si>
+    <t>Connect Camera to Arduino Board</t>
+  </si>
+  <si>
+    <t>The Arduino should be able to receive the data from the camera.</t>
+  </si>
+  <si>
+    <t>As a presenter, I want to be able to see who is at the door. (Story)</t>
+  </si>
+  <si>
+    <t>Total ideal Hours:</t>
+  </si>
+  <si>
+    <t>Storing Pictures in Database</t>
+  </si>
+  <si>
+    <t>Learn how to store pictures into a database.</t>
+  </si>
+  <si>
+    <t>BE-3.3</t>
+  </si>
+  <si>
+    <t>The presenter wants to always know if the board is connected to the phone. If it is not connected, the application will bring the presenter to another activity that will allow him/her to connect to the board.</t>
+  </si>
+  <si>
+    <t>BE-2.5</t>
+  </si>
+  <si>
+    <t>Coding Arduino Sensor</t>
+  </si>
+  <si>
+    <t>BE-2.6</t>
+  </si>
+  <si>
+    <t>Coding Arduino to send and receive signals from the sensor using thresholds.</t>
+  </si>
+  <si>
+    <t>The Arduino should be able to communicate application using Bluetooth.</t>
+  </si>
+  <si>
+    <t>Coding Arduino Camera</t>
+  </si>
+  <si>
+    <t>Coding Arduino to send and receive signals from camera.</t>
+  </si>
+  <si>
+    <t>Assigned to: Shadi Makdissi and Ogo-Oluwa Jesutomi Olasubulumi</t>
+  </si>
+  <si>
+    <t>Assigned to: Irfan Ahmed</t>
+  </si>
+  <si>
+    <t>Assigned to: Alec Kurkdjian and Cong-Vinh Vu</t>
+  </si>
+  <si>
+    <t>Assigned to: Alec Kurkdjian</t>
+  </si>
+  <si>
+    <t>Assigned to: Cong-Vinh Vu</t>
+  </si>
+  <si>
+    <t>Coding Wifi Camera</t>
+  </si>
+  <si>
+    <t>Coding Arduino to send camera pictures using Wifi.</t>
+  </si>
+  <si>
+    <t>Coding Wifi Sensor</t>
+  </si>
+  <si>
+    <t>Coding Arduino to send signals using Wfi.</t>
   </si>
 </sst>
 </file>
@@ -434,7 +595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -488,6 +649,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -549,7 +713,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -584,7 +748,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -847,10 +1011,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView topLeftCell="A22" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -860,7 +1024,7 @@
     <col min="4" max="4" width="7.44140625" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" customWidth="1"/>
     <col min="6" max="6" width="15.44140625" customWidth="1"/>
-    <col min="7" max="7" width="43.109375" customWidth="1"/>
+    <col min="7" max="7" width="46.6640625" customWidth="1"/>
     <col min="8" max="8" width="42.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -904,13 +1068,13 @@
     </row>
     <row r="6" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="C6" s="15" t="s">
         <v>23</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>24</v>
       </c>
       <c r="D6" s="3">
         <v>1</v>
@@ -922,10 +1086,10 @@
         <v>20</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -940,13 +1104,13 @@
     </row>
     <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>26</v>
-      </c>
       <c r="C8" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="3">
         <v>1</v>
@@ -958,10 +1122,10 @@
         <v>20</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -974,30 +1138,30 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="D10" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -1012,52 +1176,42 @@
     </row>
     <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B12" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>42</v>
-      </c>
       <c r="D12" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+        <v>69</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D14" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>20</v>
@@ -1066,10 +1220,10 @@
         <v>20</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -1087,13 +1241,13 @@
         <v>32</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="D16" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>20</v>
@@ -1102,10 +1256,10 @@
         <v>20</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -1120,28 +1274,28 @@
     </row>
     <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="14" t="s">
-        <v>31</v>
-      </c>
       <c r="C18" s="12" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="D18" s="2">
         <v>2</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1154,33 +1308,33 @@
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
     </row>
-    <row r="20" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>34</v>
+        <v>105</v>
       </c>
       <c r="D20" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>54</v>
+        <v>125</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="14"/>
       <c r="C21" s="12"/>
@@ -1190,33 +1344,33 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
     </row>
-    <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="D22" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="14"/>
       <c r="C23" s="12"/>
@@ -1226,92 +1380,174 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
     </row>
-    <row r="24" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="B24" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+    </row>
+    <row r="26" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="2">
+        <v>3</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+    </row>
+    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="2">
+        <v>5</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" s="2">
+      <c r="F28" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+    </row>
+    <row r="30" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="2">
         <v>3</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B25" s="14" t="s">
+      <c r="E30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="2"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+    </row>
+    <row r="32" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" s="2">
-        <v>2</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G25" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="H25" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-    </row>
-    <row r="27" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D27" s="2">
+      <c r="B32" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="2">
         <v>3</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="H27" s="14" t="s">
-        <v>77</v>
+      <c r="E32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1319,22 +1555,22 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <dataValidations count="8">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Is the task completed?" prompt="Describe the criteria to be used to determine if the task is completed as per requirements._x000a_" sqref="H5" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task status" prompt="Current status of task. One of: Planned, In Progress, On Hold, Completed" sqref="F4 F38 F40:F1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task status" prompt="Current status of task. One of: Planned, In Progress, On Hold, Completed" sqref="F35:F1048576 F33 F4" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Planned, In Progress, On Hold, Completed"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E5" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Card. One of: Planned, In Progress, On Hold, Completed" sqref="F5" xr:uid="{00000000-0002-0000-0100-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Story Point" prompt="Story point is an arbitary measure used to measure the effort required to implement a story._x000a__x000a_" sqref="D5" xr:uid="{00000000-0002-0000-0100-000004000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Priority" prompt="Priority of task. One of: Critical, High, Medium, Low" sqref="E38 E40:E1048576" xr:uid="{00000000-0002-0000-0100-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Priority" prompt="Priority of task. One of: Critical, High, Medium, Low" sqref="E33 E35:E1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Critical, High, Medium, Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Story. One of: Planned, In Progress, On Hold, Completed" sqref="F6:F27" xr:uid="{00000000-0002-0000-0100-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Story. One of: Planned, In Progress, On Hold, Completed" sqref="F6:F12 F14:F32" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Not in sprint, Sprint 1, Sprint 2, Sprint 3, In Progress, On Hold, Completed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E6:E27" xr:uid="{00000000-0002-0000-0100-000007000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E6:E12 E14:E32" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"Sprint 1, Sprint 2, Sprint 3, Future"</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Is the task completed?" prompt="Describe the criteria to be used to determine if the task is completed as per requirements._x000a_" sqref="H5" xr:uid="{00000000-0002-0000-0100-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E5" xr:uid="{00000000-0002-0000-0100-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Card. One of: Planned, In Progress, On Hold, Completed" sqref="F5" xr:uid="{00000000-0002-0000-0100-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Story Point" prompt="Story point is an arbitary measure used to measure the effort required to implement a story._x000a__x000a_" sqref="D5" xr:uid="{00000000-0002-0000-0100-000007000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="60" orientation="landscape" r:id="rId1"/>
@@ -1346,22 +1582,22 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="25.109375" customWidth="1"/>
     <col min="4" max="4" width="44.44140625" customWidth="1"/>
-    <col min="5" max="5" width="7.44140625" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" customWidth="1"/>
-    <col min="7" max="7" width="43.109375" customWidth="1"/>
+    <col min="5" max="6" width="7.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" customWidth="1"/>
+    <col min="8" max="8" width="43.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="19" t="s">
         <v>9</v>
       </c>
@@ -1371,18 +1607,30 @@
       <c r="E1" s="19"/>
       <c r="F1" s="19"/>
       <c r="G1" s="19"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="19"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
       <c r="D4" s="21"/>
       <c r="E4" s="21"/>
       <c r="F4" s="21"/>
-    </row>
-    <row r="6" spans="1:7" s="6" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="21"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" s="22"/>
+      <c r="C5">
+        <f>SUM(E7:E26)</f>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="6" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
@@ -1398,247 +1646,544 @@
       <c r="E6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="5"/>
+      <c r="G6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="3">
+        <v>3</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="3">
+        <v>5</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="3">
+        <v>3</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="3">
+        <v>5</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14" s="2">
+        <v>5</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="E15" s="2">
+        <v>5</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="D16" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="2">
+        <v>5</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="H16" s="14" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="E17" s="2">
+        <v>5</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F10" s="3" t="s">
+      <c r="H17" s="14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18" s="2">
+        <v>3</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="H18" s="14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" s="2">
+        <v>5</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F12" s="3" t="s">
+      <c r="H19" s="14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="E20" s="2">
+        <v>5</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="3" t="s">
+      <c r="H20" s="14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="E21" s="2">
+        <v>5</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="H21" s="14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="E22" s="2">
+        <v>5</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="E23" s="2">
+        <v>5</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E24" s="2">
+        <v>5</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="E25" s="2">
+        <v>5</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="E26" s="2">
+        <v>5</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>133</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A4:F4"/>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="F6" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimate" prompt="Estimated hours for the task." sqref="E6" xr:uid="{00000000-0002-0000-0200-000001000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="F7:F23" xr:uid="{00000000-0002-0000-0200-000002000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G6" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimate" prompt="Estimated hours for the task." sqref="E6:F6" xr:uid="{00000000-0002-0000-0200-000001000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G7:G26" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>"Planned, In Progress, On Hold, Completed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated Product Backlog with Priorities
</commit_message>
<xml_diff>
--- a/Documentation/Product Backlog.xlsx
+++ b/Documentation/Product Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\congv\Documents\My_Studies\Fall-2019\COEN-390\COEN-390\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E2BD1A-8DF4-4F91-9C58-BACFBC01F6E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716C541E-322A-44FA-8B97-5F517E08050A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="149">
   <si>
     <t>Story ID</t>
   </si>
@@ -170,9 +170,6 @@
   </si>
   <si>
     <t>•Display a list of all authorized users</t>
-  </si>
-  <si>
-    <t>The application monitors and registers those who have unlocked the door, it display the information once the user clicks the History button</t>
   </si>
   <si>
     <t>•Display the list of user who used the door when History is clicked</t>
@@ -448,18 +445,6 @@
     <t>Assigned to: Shadi Makdissi and Ogo-Oluwa Jesutomi Olasubulumi</t>
   </si>
   <si>
-    <t>Assigned to: Irfan Ahmed</t>
-  </si>
-  <si>
-    <t>Assigned to: Alec Kurkdjian and Cong-Vinh Vu</t>
-  </si>
-  <si>
-    <t>Assigned to: Alec Kurkdjian</t>
-  </si>
-  <si>
-    <t>Assigned to: Cong-Vinh Vu</t>
-  </si>
-  <si>
     <t>Coding Wifi Camera</t>
   </si>
   <si>
@@ -470,6 +455,51 @@
   </si>
   <si>
     <t>Coding Arduino to send signals using Wfi.</t>
+  </si>
+  <si>
+    <t>Assigned to: Irfan Ahmed
+Priority 1</t>
+  </si>
+  <si>
+    <t>Assigned to: Irfan Ahmed
+Priority 5</t>
+  </si>
+  <si>
+    <t>Assigned to: Cong-Vinh Vu
+Priority 3</t>
+  </si>
+  <si>
+    <t>Assigned to: Alec Kurkdjian
+Priority 3</t>
+  </si>
+  <si>
+    <t>Assigned to: Alec Kurkdjian
+Priority 1</t>
+  </si>
+  <si>
+    <t>Assigned to: Cong-Vinh Vu
+Priority 2</t>
+  </si>
+  <si>
+    <t>Assigned to: Alec Kurkdjian and Cong-Vinh Vu
+Priority 1</t>
+  </si>
+  <si>
+    <t>Assigned to: Alec Kurkdjian and Cong-Vinh Vu
+Priority 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assigned to: Shadi Makdissi and Ogo-Oluwa Jesutomi Olasubulumi
+</t>
+  </si>
+  <si>
+    <t>Displays pictures taken by the camera in History page.</t>
+  </si>
+  <si>
+    <t>Profile of admins should contain: username, email, password, identifier of door, and a list of admins who have access to the same door.</t>
+  </si>
+  <si>
+    <t>The presenter should be able to create a profile if they don't have one and be able to login once they have one by entering an door identifier, email address, password, and username.</t>
   </si>
 </sst>
 </file>
@@ -1086,10 +1116,10 @@
         <v>20</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1125,7 +1155,7 @@
         <v>36</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -1143,10 +1173,10 @@
         <v>29</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
@@ -1158,10 +1188,10 @@
         <v>20</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -1179,10 +1209,10 @@
         <v>28</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
@@ -1194,10 +1224,10 @@
         <v>20</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1205,7 +1235,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>42</v>
@@ -1241,10 +1271,10 @@
         <v>32</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
@@ -1256,10 +1286,10 @@
         <v>20</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -1280,7 +1310,7 @@
         <v>30</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D18" s="2">
         <v>2</v>
@@ -1292,10 +1322,10 @@
         <v>20</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1313,10 +1343,10 @@
         <v>31</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D20" s="2">
         <v>1</v>
@@ -1328,10 +1358,10 @@
         <v>20</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1349,10 +1379,10 @@
         <v>34</v>
       </c>
       <c r="B22" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="12" t="s">
         <v>86</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>87</v>
       </c>
       <c r="D22" s="2">
         <v>2</v>
@@ -1364,10 +1394,10 @@
         <v>20</v>
       </c>
       <c r="G22" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="H22" s="14" t="s">
         <v>88</v>
-      </c>
-      <c r="H22" s="14" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1382,13 +1412,13 @@
     </row>
     <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D24" s="2">
         <v>1</v>
@@ -1400,10 +1430,10 @@
         <v>20</v>
       </c>
       <c r="G24" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="H24" s="14" t="s">
         <v>109</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1418,13 +1448,13 @@
     </row>
     <row r="26" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D26" s="2">
         <v>3</v>
@@ -1454,28 +1484,28 @@
     </row>
     <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D28" s="2">
         <v>5</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -1490,28 +1520,28 @@
     </row>
     <row r="30" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D30" s="2">
         <v>3</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G30" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H30" s="14" t="s">
         <v>52</v>
-      </c>
-      <c r="H30" s="14" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -1526,10 +1556,10 @@
     </row>
     <row r="32" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>39</v>
@@ -1538,10 +1568,10 @@
         <v>3</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G32" s="14" t="s">
         <v>40</v>
@@ -1584,8 +1614,8 @@
   </sheetPr>
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1611,7 +1641,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
@@ -1622,7 +1652,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5" s="22"/>
       <c r="C5">
@@ -1662,22 +1692,22 @@
         <v>21</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E7" s="2">
         <v>2</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>134</v>
+      <c r="H7" s="14" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1697,24 +1727,24 @@
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>134</v>
+      <c r="H8" s="14" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>74</v>
-      </c>
       <c r="C9" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>43</v>
@@ -1723,16 +1753,16 @@
         <v>3</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H9" s="13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
@@ -1740,25 +1770,25 @@
         <v>32</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>45</v>
+        <v>146</v>
       </c>
       <c r="E10" s="3">
         <v>5</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
@@ -1766,48 +1796,48 @@
         <v>29</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>68</v>
+        <v>147</v>
       </c>
       <c r="E11" s="3">
         <v>3</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>70</v>
+        <v>148</v>
       </c>
       <c r="E12" s="3">
         <v>5</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1815,77 +1845,77 @@
         <v>28</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E14" s="2">
         <v>5</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C15" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D15" s="14" t="s">
         <v>122</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>123</v>
       </c>
       <c r="E15" s="2">
         <v>5</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1893,77 +1923,77 @@
         <v>34</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E16" s="2">
         <v>5</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E17" s="2">
         <v>5</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C18" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" s="14" t="s">
         <v>103</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>104</v>
       </c>
       <c r="E18" s="2">
         <v>3</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1971,25 +2001,25 @@
         <v>33</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C19" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" s="14" t="s">
         <v>92</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>93</v>
       </c>
       <c r="E19" s="2">
         <v>5</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1997,25 +2027,25 @@
         <v>33</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E20" s="2">
         <v>5</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2023,25 +2053,25 @@
         <v>33</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E21" s="2">
         <v>5</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2049,25 +2079,25 @@
         <v>33</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E22" s="2">
         <v>5</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -2078,100 +2108,100 @@
         <v>31</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E23" s="2">
         <v>5</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C24" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" s="14" t="s">
         <v>118</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>119</v>
       </c>
       <c r="E24" s="2">
         <v>5</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C25" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D25" s="14" t="s">
         <v>131</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>132</v>
       </c>
       <c r="E25" s="2">
         <v>5</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E26" s="2">
         <v>5</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Updated Product Backlog with Priorities"
This reverts commit 75f8456ccb97b9e6b7a491f77792eacd53670bd9.
</commit_message>
<xml_diff>
--- a/Documentation/Product Backlog.xlsx
+++ b/Documentation/Product Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\congv\Documents\My_Studies\Fall-2019\COEN-390\COEN-390\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716C541E-322A-44FA-8B97-5F517E08050A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E2BD1A-8DF4-4F91-9C58-BACFBC01F6E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="142">
   <si>
     <t>Story ID</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t>•Display a list of all authorized users</t>
+  </si>
+  <si>
+    <t>The application monitors and registers those who have unlocked the door, it display the information once the user clicks the History button</t>
   </si>
   <si>
     <t>•Display the list of user who used the door when History is clicked</t>
@@ -445,6 +448,18 @@
     <t>Assigned to: Shadi Makdissi and Ogo-Oluwa Jesutomi Olasubulumi</t>
   </si>
   <si>
+    <t>Assigned to: Irfan Ahmed</t>
+  </si>
+  <si>
+    <t>Assigned to: Alec Kurkdjian and Cong-Vinh Vu</t>
+  </si>
+  <si>
+    <t>Assigned to: Alec Kurkdjian</t>
+  </si>
+  <si>
+    <t>Assigned to: Cong-Vinh Vu</t>
+  </si>
+  <si>
     <t>Coding Wifi Camera</t>
   </si>
   <si>
@@ -455,51 +470,6 @@
   </si>
   <si>
     <t>Coding Arduino to send signals using Wfi.</t>
-  </si>
-  <si>
-    <t>Assigned to: Irfan Ahmed
-Priority 1</t>
-  </si>
-  <si>
-    <t>Assigned to: Irfan Ahmed
-Priority 5</t>
-  </si>
-  <si>
-    <t>Assigned to: Cong-Vinh Vu
-Priority 3</t>
-  </si>
-  <si>
-    <t>Assigned to: Alec Kurkdjian
-Priority 3</t>
-  </si>
-  <si>
-    <t>Assigned to: Alec Kurkdjian
-Priority 1</t>
-  </si>
-  <si>
-    <t>Assigned to: Cong-Vinh Vu
-Priority 2</t>
-  </si>
-  <si>
-    <t>Assigned to: Alec Kurkdjian and Cong-Vinh Vu
-Priority 1</t>
-  </si>
-  <si>
-    <t>Assigned to: Alec Kurkdjian and Cong-Vinh Vu
-Priority 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assigned to: Shadi Makdissi and Ogo-Oluwa Jesutomi Olasubulumi
-</t>
-  </si>
-  <si>
-    <t>Displays pictures taken by the camera in History page.</t>
-  </si>
-  <si>
-    <t>Profile of admins should contain: username, email, password, identifier of door, and a list of admins who have access to the same door.</t>
-  </si>
-  <si>
-    <t>The presenter should be able to create a profile if they don't have one and be able to login once they have one by entering an door identifier, email address, password, and username.</t>
   </si>
 </sst>
 </file>
@@ -1116,10 +1086,10 @@
         <v>20</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1155,7 +1125,7 @@
         <v>36</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -1173,10 +1143,10 @@
         <v>29</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
@@ -1188,10 +1158,10 @@
         <v>20</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -1209,10 +1179,10 @@
         <v>28</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
@@ -1224,10 +1194,10 @@
         <v>20</v>
       </c>
       <c r="G12" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" s="14" t="s">
         <v>69</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1235,7 +1205,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>42</v>
@@ -1271,10 +1241,10 @@
         <v>32</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
@@ -1286,10 +1256,10 @@
         <v>20</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -1310,7 +1280,7 @@
         <v>30</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D18" s="2">
         <v>2</v>
@@ -1322,10 +1292,10 @@
         <v>20</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1343,10 +1313,10 @@
         <v>31</v>
       </c>
       <c r="B20" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>105</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>104</v>
       </c>
       <c r="D20" s="2">
         <v>1</v>
@@ -1358,10 +1328,10 @@
         <v>20</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1379,10 +1349,10 @@
         <v>34</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D22" s="2">
         <v>2</v>
@@ -1394,10 +1364,10 @@
         <v>20</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1412,13 +1382,13 @@
     </row>
     <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D24" s="2">
         <v>1</v>
@@ -1430,10 +1400,10 @@
         <v>20</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1448,13 +1418,13 @@
     </row>
     <row r="26" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D26" s="2">
         <v>3</v>
@@ -1484,28 +1454,28 @@
     </row>
     <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D28" s="2">
         <v>5</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -1520,28 +1490,28 @@
     </row>
     <row r="30" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D30" s="2">
         <v>3</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -1556,10 +1526,10 @@
     </row>
     <row r="32" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>39</v>
@@ -1568,10 +1538,10 @@
         <v>3</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G32" s="14" t="s">
         <v>40</v>
@@ -1614,8 +1584,8 @@
   </sheetPr>
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1641,7 +1611,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
@@ -1652,7 +1622,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B5" s="22"/>
       <c r="C5">
@@ -1692,22 +1662,22 @@
         <v>21</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E7" s="2">
         <v>2</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="14" t="s">
-        <v>137</v>
+      <c r="H7" s="2" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1727,24 +1697,24 @@
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="14" t="s">
-        <v>138</v>
+      <c r="H8" s="2" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>43</v>
@@ -1753,16 +1723,16 @@
         <v>3</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="13" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H9" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
@@ -1770,25 +1740,25 @@
         <v>32</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>146</v>
+        <v>45</v>
       </c>
       <c r="E10" s="3">
         <v>5</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
@@ -1796,48 +1766,48 @@
         <v>29</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>147</v>
+        <v>68</v>
       </c>
       <c r="E11" s="3">
         <v>3</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>148</v>
+        <v>70</v>
       </c>
       <c r="E12" s="3">
         <v>5</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1845,77 +1815,77 @@
         <v>28</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E14" s="2">
         <v>5</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E15" s="2">
         <v>5</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1923,77 +1893,77 @@
         <v>34</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E16" s="2">
         <v>5</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E17" s="2">
         <v>5</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E18" s="2">
         <v>3</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2001,25 +1971,25 @@
         <v>33</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E19" s="2">
         <v>5</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2027,25 +1997,25 @@
         <v>33</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E20" s="2">
         <v>5</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2053,25 +2023,25 @@
         <v>33</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E21" s="2">
         <v>5</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2079,25 +2049,25 @@
         <v>33</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="E22" s="2">
         <v>5</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -2108,100 +2078,100 @@
         <v>31</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E23" s="2">
         <v>5</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E24" s="2">
         <v>5</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E25" s="2">
         <v>5</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="E26" s="2">
         <v>5</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated product backlog and adding backbone for sprint 2
</commit_message>
<xml_diff>
--- a/Documentation/Product Backlog.xlsx
+++ b/Documentation/Product Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irfan Ahmed\AndroidStudioProjects\ELEC-COEN-390\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomil\StudioProjects\ELEC-COEN-390\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C0A62C-D5DF-4288-8725-80E265C4F156}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962BC2CD-951A-43E7-B7A9-50779A85EBBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,14 +37,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="177">
   <si>
     <t>Story ID</t>
   </si>
   <si>
-    <t>Story Points</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -140,9 +139,6 @@
   </si>
   <si>
     <t>BE-3</t>
-  </si>
-  <si>
-    <t>Sprint 2</t>
   </si>
   <si>
     <t>The credit button will lead the presenter to another activity containing the information regarding the collaborators of the application</t>
@@ -216,9 +212,6 @@
     <t>Open Door Button</t>
   </si>
   <si>
-    <t>Sprint 3</t>
-  </si>
-  <si>
     <t>Main Page Button</t>
   </si>
   <si>
@@ -229,12 +222,6 @@
   </si>
   <si>
     <t>Login Page</t>
-  </si>
-  <si>
-    <t>As a presenter, I want to be able to create a profile (Story)</t>
-  </si>
-  <si>
-    <t>As a presenter, I want to be able to login (Story)</t>
   </si>
   <si>
     <t>The presenter should be able to create a profile.</t>
@@ -289,16 +276,10 @@
     <t>The application monitors and registers those who have unlocked the door, it display the pictures took once the user clicks the History button</t>
   </si>
   <si>
-    <t>Sprint 1 Goal(s): Finish the back-end, front-end of the project</t>
-  </si>
-  <si>
     <t>There will be 5 buttons on the main page. The first one will allow the user to check the what is in front of the door, the second will be used to open a door, the third will be used to to show the user who has access to the door. The fourth used to see who last used the door and finally the last button shows the application credits. (See Documentation/Layout_Pictures/main_page)</t>
   </si>
   <si>
     <t>Setup Database</t>
-  </si>
-  <si>
-    <t>As a user, I want my profile to be saved (Story)</t>
   </si>
   <si>
     <t>The user's profile should be saved in a database, using Firebase.</t>
@@ -516,6 +497,99 @@
   <si>
     <t xml:space="preserve">Assigned to: Shadi Makdissi , Ogo-Oluwa Jesutomi Olasubulumi and Irfan Ahmed
 </t>
+  </si>
+  <si>
+    <t>EX-1</t>
+  </si>
+  <si>
+    <t>Gesture</t>
+  </si>
+  <si>
+    <t>A a user I want to be able to open the door using a gesture sensor using bluetooth and within a close range</t>
+  </si>
+  <si>
+    <t>EX -2</t>
+  </si>
+  <si>
+    <t>Face Recognition</t>
+  </si>
+  <si>
+    <t>As a admin, I want the app to scan the picture of me it took at the door so that it verifies that I am an admin and unlock the door automatically for me</t>
+  </si>
+  <si>
+    <t>•The pictures taken are scanned
+•The software distinguishes an admin from others
+•The only opens for admin after verification</t>
+  </si>
+  <si>
+    <t>•The door opens with gestures</t>
+  </si>
+  <si>
+    <t>Not in sprint</t>
+  </si>
+  <si>
+    <t>As a user, I want my admin profile, history, and pictures to be saved on database so that I can easily access them anywhere</t>
+  </si>
+  <si>
+    <t>Story Points/Size</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Future</t>
+  </si>
+  <si>
+    <t>The camera takes picture of the person at the door and scans if it is an admin</t>
+  </si>
+  <si>
+    <t>The gesture sensor opens the door for the user when used</t>
+  </si>
+  <si>
+    <t>Sprint 1 Goal(s): Finish the App skeleton,Create database server, Coding and Testing of sensor for arduino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 1 Goal(s): </t>
+  </si>
+  <si>
+    <t>Sprint 2 Backlog</t>
+  </si>
+  <si>
+    <t>As a presenter, I want to be able to create a profile so that I can add a user as an admin(story)</t>
+  </si>
+  <si>
+    <t>As a presenter, I want to be able to login so that I can check who has access to the door(Story)</t>
+  </si>
+  <si>
+    <t>EX-3</t>
+  </si>
+  <si>
+    <t>Accessing history requires password</t>
+  </si>
+  <si>
+    <t>As an admin I want the app to only let admin users access history page by requesting for password to open the door</t>
+  </si>
+  <si>
+    <t>The app only access users who have admin priviledges to view history</t>
+  </si>
+  <si>
+    <t>•Password is requested when the history button is pressed
+•The history page is open once ocrect password is inputted</t>
+  </si>
+  <si>
+    <t>EX-4</t>
+  </si>
+  <si>
+    <t>Monitor who opens the door for who</t>
+  </si>
+  <si>
+    <t>As an admin I want the the history page to also record the user's device that open the door so that I can monitor which admin opens the door</t>
+  </si>
+  <si>
+    <t>•The history page shows the admin who opened the door along with the user that was at the door</t>
+  </si>
+  <si>
+    <t>The app shows which admin opened the door</t>
   </si>
 </sst>
 </file>
@@ -700,6 +774,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -710,7 +785,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -997,67 +1071,67 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="126.7109375" customWidth="1"/>
+    <col min="1" max="1" width="126.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="7" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:1" s="7" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" s="7" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:1" s="7" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A3" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:1" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A8" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:1" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:1" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:1" s="11" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" s="11" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" s="11" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="17" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="18" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="19" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="21" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="22" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="23" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="24" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="25" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="26" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="27" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="28" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="29" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="30" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -1069,88 +1143,88 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="93" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="44.42578125" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="46.7109375" customWidth="1"/>
-    <col min="8" max="8" width="42.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="44.44140625" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1"/>
+    <col min="7" max="7" width="46.6640625" customWidth="1"/>
+    <col min="8" max="8" width="42.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-    </row>
-    <row r="5" spans="1:8" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+    </row>
+    <row r="5" spans="1:8" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="16" t="s">
+      <c r="F5" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="C6" s="15" t="s">
         <v>22</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>23</v>
       </c>
       <c r="D6" s="3">
         <v>1</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>20</v>
+        <v>158</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -1160,33 +1234,33 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="C8" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="3">
         <v>1</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>20</v>
+        <v>158</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="14"/>
       <c r="C9" s="12"/>
@@ -1196,33 +1270,33 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>64</v>
+        <v>165</v>
       </c>
       <c r="D10" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>20</v>
+        <v>158</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="14"/>
       <c r="C11" s="12"/>
@@ -1232,59 +1306,59 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G12" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" s="2">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>68</v>
-      </c>
       <c r="H12" s="14" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C14" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="2">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="2">
-        <v>1</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="14"/>
       <c r="C15" s="12"/>
@@ -1294,33 +1368,33 @@
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
     </row>
-    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D16" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>20</v>
+        <v>158</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="14"/>
       <c r="C17" s="12"/>
@@ -1330,33 +1404,33 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
     </row>
-    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D18" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>20</v>
+        <v>158</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="14"/>
       <c r="C19" s="12"/>
@@ -1366,33 +1440,33 @@
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
     </row>
-    <row r="20" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>102</v>
+        <v>156</v>
       </c>
       <c r="D20" s="2">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>20</v>
+        <v>158</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>121</v>
+        <v>79</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="14"/>
       <c r="C21" s="12"/>
@@ -1402,33 +1476,33 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
     </row>
-    <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="D22" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>20</v>
+        <v>159</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>20</v>
+        <v>155</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="14"/>
       <c r="C23" s="12"/>
@@ -1438,33 +1512,33 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
     </row>
-    <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D24" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>20</v>
+        <v>159</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>20</v>
+        <v>155</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="14"/>
       <c r="C25" s="12"/>
@@ -1474,33 +1548,33 @@
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
     </row>
-    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B26" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>48</v>
       </c>
       <c r="D26" s="2">
         <v>3</v>
       </c>
       <c r="E26" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G26" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G26" s="14" t="s">
-        <v>37</v>
-      </c>
       <c r="H26" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="14"/>
       <c r="C27" s="12"/>
@@ -1510,33 +1584,33 @@
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
     </row>
-    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D28" s="2">
         <v>5</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="14"/>
       <c r="C29" s="12"/>
@@ -1546,33 +1620,33 @@
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
     </row>
-    <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C30" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="2">
+        <v>2</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="H30" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D30" s="2">
-        <v>3</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G30" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="H30" s="14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="14"/>
       <c r="C31" s="12"/>
@@ -1582,30 +1656,164 @@
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
     </row>
-    <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D32" s="2">
         <v>3</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
       <c r="G32" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H32" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="2"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+    </row>
+    <row r="34" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="D34" s="2">
+        <v>13</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G34" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="H34" s="14" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="2"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+    </row>
+    <row r="36" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D36" s="2">
+        <v>21</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G36" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="H36" s="14" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+    </row>
+    <row r="38" spans="1:8" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="D38" s="2">
+        <v>5</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G38" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="H38" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="D40" s="2">
+        <v>3</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G40" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="H40" s="14" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -1613,16 +1821,16 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task status" prompt="Current status of task. One of: Planned, In Progress, On Hold, Completed" sqref="F35:F1048576 F33 F4" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task status" prompt="Current status of task. One of: Planned, In Progress, On Hold, Completed" sqref="F41:F1048576 F39 F4" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Planned, In Progress, On Hold, Completed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Priority" prompt="Priority of task. One of: Critical, High, Medium, Low" sqref="E33 E35:E1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Priority" prompt="Priority of task. One of: Critical, High, Medium, Low" sqref="E39 E41:E1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Critical, High, Medium, Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Story. One of: Planned, In Progress, On Hold, Completed" sqref="F6:F12 F14:F32" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Story. One of: Planned, In Progress, On Hold, Completed" sqref="F6:F12 F14:F38 F40" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Not in sprint, Sprint 1, Sprint 2, Sprint 3, In Progress, On Hold, Completed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E6:E12 E14:E32" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E6:E12 E14:E38 E40" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"Sprint 1, Sprint 2, Sprint 3, Future"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Is the task completed?" prompt="Describe the criteria to be used to determine if the task is completed as per requirements._x000a_" sqref="H5" xr:uid="{00000000-0002-0000-0100-000004000000}"/>
@@ -1642,624 +1850,624 @@
   </sheetPr>
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="25.140625" customWidth="1"/>
-    <col min="4" max="4" width="44.42578125" customWidth="1"/>
-    <col min="5" max="6" width="7.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="43.140625" customWidth="1"/>
+    <col min="3" max="3" width="25.109375" customWidth="1"/>
+    <col min="4" max="4" width="44.44140625" customWidth="1"/>
+    <col min="5" max="6" width="7.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" customWidth="1"/>
+    <col min="8" max="8" width="43.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="B5" s="22"/>
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" s="23"/>
       <c r="C5">
         <f>SUM(E7:E27)</f>
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="6" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="6" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E7" s="2">
         <v>2</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>25</v>
-      </c>
       <c r="D8" s="18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E8" s="2">
         <v>2</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E9" s="3">
         <v>3</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H9" s="13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>141</v>
       </c>
       <c r="E10" s="3">
         <v>5</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H10" s="14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="18" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>142</v>
       </c>
       <c r="E11" s="3">
         <v>3</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H11" s="14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="13" t="s">
         <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>143</v>
       </c>
       <c r="E12" s="3">
         <v>5</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E14" s="2">
         <v>5</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E15" s="2">
         <v>5</v>
       </c>
       <c r="F15" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>120</v>
-      </c>
       <c r="C16" s="14" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E16" s="2">
         <v>5</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E17" s="2">
         <v>5</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="E18" s="2">
         <v>5</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="E19" s="2">
         <v>5</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E20" s="2">
         <v>5</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E21" s="2">
         <v>5</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="E22" s="2">
         <v>5</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E23" s="2">
         <v>5</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="E24" s="2">
         <v>5</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="E25" s="2">
         <v>5</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="E26" s="2">
         <v>5</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E27" s="2">
         <v>5</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H27" s="14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2281,14 +2489,302 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5">
+        <f>SUM(E7:E27)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="14"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="14"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="14"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="14"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="13"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="13"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="14"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="14"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="14"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="14"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="14"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="14"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="14"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="14"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="14"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="14"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="14"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="14"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:B5"/>
+  </mergeCells>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G7:G27" xr:uid="{E867160D-44FB-45CD-9210-A1CD3453DD81}">
+      <formula1>"Planned, In Progress, On Hold, Completed"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimate" prompt="Estimated hours for the task." sqref="E6:F6" xr:uid="{ED4CD34B-60FD-4426-92D6-627FAEC01E54}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G6" xr:uid="{1D6B67AD-7355-44D9-982C-EFD8A38C1E19}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2300,7 +2796,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Sprint 2 Backlog Corrections
-Made the sprint 2 goal less vague
-Minor correction to product backlog and sprint 2
</commit_message>
<xml_diff>
--- a/Documentation/Product Backlog.xlsx
+++ b/Documentation/Product Backlog.xlsx
@@ -14,7 +14,6 @@
     <sheet name="Sprint 3" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -799,9 +798,6 @@
     <t>Create a  profile page and allow user to modify their credentials.</t>
   </si>
   <si>
-    <t>Sprint 2 Goal(s): Communication with Database and Finish Back-End Heavy Tasks</t>
-  </si>
-  <si>
     <t>Shadi Makdissi: 40060588</t>
   </si>
   <si>
@@ -946,6 +942,9 @@
   </si>
   <si>
     <t>BE-4.3</t>
+  </si>
+  <si>
+    <t>Sprint 2 Goal(s): Hardware Communication with Database and Finish Login Page, History Page, Administartors Page and, Start Peek Door</t>
   </si>
 </sst>
 </file>
@@ -1071,7 +1070,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1148,6 +1147,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1421,7 +1423,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1465,27 +1467,27 @@
     <row r="9" spans="1:1" s="7" customFormat="1"/>
     <row r="10" spans="1:1" s="11" customFormat="1" ht="18.75">
       <c r="A10" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:1" s="11" customFormat="1" ht="18.75">
       <c r="A11" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:1" s="11" customFormat="1" ht="18.75">
       <c r="A12" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="13" spans="1:1" s="7" customFormat="1" ht="18.75">
       <c r="A13" s="10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="14" spans="1:1" s="7" customFormat="1" ht="18.75">
       <c r="A14" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="15" spans="1:1" s="7" customFormat="1"/>
@@ -1515,10 +1517,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView topLeftCell="A45" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1963,10 +1965,10 @@
         <v>27</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D27" s="20">
         <v>8</v>
@@ -2238,28 +2240,28 @@
     </row>
     <row r="43" spans="1:8" ht="60">
       <c r="A43" s="20" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>128</v>
+        <v>178</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D43" s="20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E43" s="20" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>204</v>
+        <v>179</v>
       </c>
       <c r="H43" s="15" t="s">
-        <v>205</v>
+        <v>235</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2272,15 +2274,15 @@
       <c r="G44" s="15"/>
       <c r="H44" s="15"/>
     </row>
-    <row r="45" spans="1:8" ht="45">
+    <row r="45" spans="1:8" ht="60">
       <c r="A45" s="20" t="s">
-        <v>129</v>
+        <v>54</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>36</v>
+        <v>128</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D45" s="20">
         <v>2</v>
@@ -2292,10 +2294,10 @@
         <v>112</v>
       </c>
       <c r="G45" s="15" t="s">
-        <v>35</v>
+        <v>204</v>
       </c>
       <c r="H45" s="15" t="s">
-        <v>130</v>
+        <v>205</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2308,18 +2310,18 @@
       <c r="G46" s="15"/>
       <c r="H46" s="15"/>
     </row>
-    <row r="47" spans="1:8" ht="60">
+    <row r="47" spans="1:8" ht="45">
       <c r="A47" s="20" t="s">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D47" s="20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E47" s="20" t="s">
         <v>115</v>
@@ -2328,10 +2330,10 @@
         <v>112</v>
       </c>
       <c r="G47" s="15" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H47" s="15" t="s">
-        <v>231</v>
+        <v>130</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -2346,16 +2348,16 @@
     </row>
     <row r="49" spans="1:8" ht="60">
       <c r="A49" s="20" t="s">
-        <v>109</v>
+        <v>49</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>110</v>
+        <v>41</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D49" s="20">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E49" s="20" t="s">
         <v>115</v>
@@ -2364,10 +2366,10 @@
         <v>112</v>
       </c>
       <c r="G49" s="15" t="s">
-        <v>117</v>
+        <v>32</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -2382,16 +2384,16 @@
     </row>
     <row r="51" spans="1:8" ht="60">
       <c r="A51" s="20" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>154</v>
+        <v>110</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>203</v>
+        <v>225</v>
       </c>
       <c r="D51" s="20">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E51" s="20" t="s">
         <v>115</v>
@@ -2400,10 +2402,10 @@
         <v>112</v>
       </c>
       <c r="G51" s="15" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H51" s="15" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -2418,16 +2420,16 @@
     </row>
     <row r="53" spans="1:8" ht="60">
       <c r="A53" s="20" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>226</v>
+        <v>203</v>
       </c>
       <c r="D53" s="20">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E53" s="20" t="s">
         <v>115</v>
@@ -2436,10 +2438,10 @@
         <v>112</v>
       </c>
       <c r="G53" s="15" t="s">
-        <v>227</v>
+        <v>116</v>
       </c>
       <c r="H53" s="15" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -2454,45 +2456,55 @@
     </row>
     <row r="55" spans="1:8" ht="58.15" customHeight="1">
       <c r="A55" s="20" t="s">
-        <v>48</v>
+        <v>119</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>178</v>
+        <v>153</v>
       </c>
       <c r="C55" s="21" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="D55" s="20">
         <v>3</v>
       </c>
       <c r="E55" s="20" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="F55" s="20" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G55" s="15" t="s">
-        <v>179</v>
+        <v>227</v>
       </c>
       <c r="H55" s="15" t="s">
-        <v>235</v>
-      </c>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="20"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task status" prompt="Current status of task. One of: Planned, In Progress, On Hold, Completed" sqref="F4 F56:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task status" prompt="Current status of task. One of: Planned, In Progress, On Hold, Completed" sqref="F57:F1048576 F4">
       <formula1>"Planned, In Progress, On Hold, Completed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Priority" prompt="Priority of task. One of: Critical, High, Medium, Low" sqref="E56:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Priority" prompt="Priority of task. One of: Critical, High, Medium, Low" sqref="E57:E1048576">
       <formula1>"Critical, High, Medium, Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Story. One of: Planned, In Progress, On Hold, Completed" sqref="F33:F55 F6:F29 F30:F31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Story. One of: Planned, In Progress, On Hold, Completed" sqref="F6:F31 F33:F56">
       <formula1>"Not in sprint, Sprint 1, Sprint 2, Sprint 3, In Progress, On Hold, Completed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E33:E55 E6:E29 E30:E31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E6:E31 E33:E56">
       <formula1>"Sprint 1, Sprint 2, Sprint 3, Future"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Is the task completed?" prompt="Describe the criteria to be used to determine if the task is completed as per requirements.&#10;" sqref="H5"/>
@@ -2539,7 +2551,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="27" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B4" s="27"/>
       <c r="C4" s="27"/>
@@ -2605,7 +2617,7 @@
         <v>120</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="60">
@@ -2631,7 +2643,7 @@
         <v>120</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="60">
@@ -2657,7 +2669,7 @@
         <v>120</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="60">
@@ -2683,7 +2695,7 @@
         <v>120</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="60">
@@ -2709,7 +2721,7 @@
         <v>120</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="75">
@@ -2735,7 +2747,7 @@
         <v>120</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="45">
@@ -2761,7 +2773,7 @@
         <v>120</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="60">
@@ -2787,7 +2799,7 @@
         <v>120</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="75">
@@ -2813,7 +2825,7 @@
         <v>120</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="45">
@@ -2839,7 +2851,7 @@
         <v>120</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="60">
@@ -2865,7 +2877,7 @@
         <v>120</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="45">
@@ -2891,7 +2903,7 @@
         <v>120</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="45">
@@ -2917,7 +2929,7 @@
         <v>120</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="45">
@@ -2943,7 +2955,7 @@
         <v>120</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="45">
@@ -2969,7 +2981,7 @@
         <v>120</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="60">
@@ -2995,7 +3007,7 @@
         <v>120</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="30">
@@ -3003,13 +3015,13 @@
         <v>43</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>108</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E23" s="2">
         <v>5</v>
@@ -3021,7 +3033,7 @@
         <v>120</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="45">
@@ -3047,7 +3059,7 @@
         <v>120</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -3072,8 +3084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3098,16 +3110,17 @@
       <c r="G1" s="26"/>
       <c r="H1" s="26"/>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="27" t="s">
-        <v>249</v>
-      </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
+    <row r="4" spans="1:8" ht="15" customHeight="1">
+      <c r="A4" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="28" t="s">
@@ -3116,7 +3129,7 @@
       <c r="B5" s="28"/>
       <c r="C5">
         <f>SUM(E3:E31)</f>
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30">
@@ -3166,7 +3179,7 @@
         <v>15</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="60">
@@ -3287,7 +3300,7 @@
         <v>192</v>
       </c>
       <c r="E12" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>80</v>
@@ -3374,7 +3387,7 @@
         <v>15</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="45">
@@ -3426,7 +3439,7 @@
         <v>15</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="60">
@@ -3452,7 +3465,7 @@
         <v>15</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="45">
@@ -3478,7 +3491,7 @@
         <v>15</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="60">
@@ -3504,7 +3517,7 @@
         <v>15</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="60">
@@ -3515,10 +3528,10 @@
         <v>27</v>
       </c>
       <c r="C21" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="D21" s="13" t="s">
         <v>262</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>263</v>
       </c>
       <c r="E21" s="2">
         <v>5</v>
@@ -3530,7 +3543,7 @@
         <v>15</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="87" customHeight="1">
@@ -3608,7 +3621,7 @@
         <v>15</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="45" customHeight="1">
@@ -3634,7 +3647,7 @@
         <v>15</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="45">
@@ -3660,7 +3673,7 @@
         <v>15</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="45">
@@ -3686,7 +3699,7 @@
         <v>15</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="30">
@@ -3738,7 +3751,7 @@
         <v>15</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="45">
@@ -3794,8 +3807,8 @@
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A4:G4"/>
     <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:H4"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G7:G31">

</xml_diff>

<commit_message>
addede 3d files and an rough idea to backlog
</commit_message>
<xml_diff>
--- a/Documentation/Product Backlog.xlsx
+++ b/Documentation/Product Backlog.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22215"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomil\StudioProjects\ELEC-COEN-390\Documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CAE12F1-7AAC-40DF-A3E9-D0FBF1A13BD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19335" windowHeight="7560" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="5" r:id="rId1"/>
@@ -13,15 +19,17 @@
     <sheet name="Sprint 2" sheetId="3" r:id="rId4"/>
     <sheet name="Sprint 3" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="288">
   <si>
     <t>Story ID</t>
   </si>
@@ -946,12 +954,15 @@
   <si>
     <t>Sprint 2 Goal(s): Hardware Communication with Database and Finish Login Page, History Page, Administartors Page and, Start Peek Door</t>
   </si>
+  <si>
+    <t>RFID</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1423,89 +1434,89 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="126.7109375" customWidth="1"/>
+    <col min="1" max="1" width="126.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="7" customFormat="1" ht="13.5" customHeight="1"/>
-    <row r="2" spans="1:1" s="7" customFormat="1"/>
-    <row r="3" spans="1:1" s="7" customFormat="1" ht="26.25">
+    <row r="1" spans="1:1" s="7" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:1" s="7" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A3" s="8" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="7" customFormat="1"/>
-    <row r="5" spans="1:1" s="7" customFormat="1"/>
-    <row r="6" spans="1:1" s="7" customFormat="1" ht="21">
+    <row r="4" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:1" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="7" customFormat="1">
+    <row r="7" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:1" s="7" customFormat="1" ht="21">
+    <row r="8" spans="1:1" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A8" s="9" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:1" s="7" customFormat="1"/>
-    <row r="10" spans="1:1" s="11" customFormat="1" ht="18.75">
+    <row r="9" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:1" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="11" spans="1:1" s="11" customFormat="1" ht="18.75">
+    <row r="11" spans="1:1" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="1:1" s="11" customFormat="1" ht="18.75">
+    <row r="12" spans="1:1" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="13" spans="1:1" s="7" customFormat="1" ht="18.75">
+    <row r="13" spans="1:1" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="14" spans="1:1" s="7" customFormat="1" ht="18.75">
+    <row r="14" spans="1:1" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="15" spans="1:1" s="7" customFormat="1"/>
-    <row r="16" spans="1:1" s="7" customFormat="1"/>
-    <row r="17" s="7" customFormat="1"/>
-    <row r="18" s="7" customFormat="1"/>
-    <row r="19" s="7" customFormat="1"/>
-    <row r="20" s="7" customFormat="1"/>
-    <row r="21" s="7" customFormat="1"/>
-    <row r="22" s="7" customFormat="1"/>
-    <row r="23" s="7" customFormat="1"/>
-    <row r="24" s="7" customFormat="1"/>
-    <row r="25" s="7" customFormat="1"/>
-    <row r="26" s="7" customFormat="1"/>
-    <row r="27" s="7" customFormat="1"/>
-    <row r="28" s="7" customFormat="1"/>
-    <row r="29" s="7" customFormat="1"/>
-    <row r="30" s="7" customFormat="1"/>
+    <row r="15" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="17" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="18" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="19" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="21" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="22" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="23" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="24" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="25" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="26" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="27" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="28" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="29" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="30" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -1513,30 +1524,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="16"/>
-    <col min="2" max="2" width="18.42578125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="44.42578125" style="16" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="16" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="16" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="46.7109375" style="16" customWidth="1"/>
-    <col min="8" max="8" width="42.5703125" style="16" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="16"/>
+    <col min="1" max="1" width="8.88671875" style="16"/>
+    <col min="2" max="2" width="18.44140625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="44.44140625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="16" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" style="16" customWidth="1"/>
+    <col min="7" max="7" width="46.6640625" style="16" customWidth="1"/>
+    <col min="8" max="8" width="42.5546875" style="16" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="24" t="s">
         <v>4</v>
       </c>
@@ -1548,7 +1559,7 @@
       <c r="G1" s="25"/>
       <c r="H1" s="25"/>
     </row>
-    <row r="5" spans="1:8" s="23" customFormat="1" ht="40.5" customHeight="1">
+    <row r="5" spans="1:8" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>0</v>
       </c>
@@ -1574,7 +1585,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="120">
+    <row r="6" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>17</v>
       </c>
@@ -1600,7 +1611,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="20"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
@@ -1610,7 +1621,7 @@
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
     </row>
-    <row r="8" spans="1:8" ht="60">
+    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>20</v>
       </c>
@@ -1636,7 +1647,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="20"/>
       <c r="B9" s="15"/>
       <c r="C9" s="21"/>
@@ -1646,7 +1657,7 @@
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
     </row>
-    <row r="10" spans="1:8" ht="30">
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>25</v>
       </c>
@@ -1672,7 +1683,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="20"/>
       <c r="B11" s="15"/>
       <c r="C11" s="21"/>
@@ -1682,7 +1693,7 @@
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
     </row>
-    <row r="12" spans="1:8" ht="45">
+    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>24</v>
       </c>
@@ -1708,7 +1719,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="45">
+    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>28</v>
       </c>
@@ -1734,7 +1745,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="20"/>
       <c r="B14" s="15"/>
       <c r="C14" s="21"/>
@@ -1744,7 +1755,7 @@
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
     </row>
-    <row r="15" spans="1:8" ht="45">
+    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>30</v>
       </c>
@@ -1770,7 +1781,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="20"/>
       <c r="B16" s="15"/>
       <c r="C16" s="21"/>
@@ -1780,7 +1791,7 @@
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
     </row>
-    <row r="17" spans="1:8" ht="60">
+    <row r="17" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>144</v>
       </c>
@@ -1806,7 +1817,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="20"/>
       <c r="B18" s="15"/>
       <c r="C18" s="21"/>
@@ -1816,7 +1827,7 @@
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
     </row>
-    <row r="19" spans="1:8" ht="45">
+    <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>147</v>
       </c>
@@ -1842,7 +1853,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.6" customHeight="1">
+    <row r="20" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="20"/>
       <c r="B20" s="15"/>
       <c r="C20" s="21"/>
@@ -1852,7 +1863,7 @@
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
     </row>
-    <row r="21" spans="1:8" ht="56.45" customHeight="1">
+    <row r="21" spans="1:8" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>156</v>
       </c>
@@ -1878,7 +1889,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="19.149999999999999" customHeight="1">
+    <row r="22" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="20"/>
       <c r="B22" s="15"/>
       <c r="C22" s="21"/>
@@ -1888,7 +1899,7 @@
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
     </row>
-    <row r="23" spans="1:8" ht="61.9" customHeight="1">
+    <row r="23" spans="1:8" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>157</v>
       </c>
@@ -1914,7 +1925,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="17.45" customHeight="1">
+    <row r="24" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="20"/>
       <c r="B24" s="15"/>
       <c r="C24" s="21"/>
@@ -1924,7 +1935,7 @@
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
     </row>
-    <row r="25" spans="1:8" ht="56.45" customHeight="1">
+    <row r="25" spans="1:8" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>29</v>
       </c>
@@ -1950,7 +1961,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="20"/>
       <c r="B26" s="15"/>
       <c r="C26" s="21"/>
@@ -1960,7 +1971,7 @@
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
     </row>
-    <row r="27" spans="1:8" ht="56.45" customHeight="1">
+    <row r="27" spans="1:8" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
         <v>27</v>
       </c>
@@ -1986,7 +1997,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="20"/>
       <c r="B28" s="15"/>
       <c r="C28" s="21"/>
@@ -1996,7 +2007,7 @@
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
     </row>
-    <row r="29" spans="1:8" ht="45">
+    <row r="29" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>43</v>
       </c>
@@ -2022,7 +2033,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="21" customHeight="1">
+    <row r="30" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="20"/>
       <c r="B30" s="15"/>
       <c r="C30" s="21"/>
@@ -2032,7 +2043,7 @@
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>
     </row>
-    <row r="31" spans="1:8" ht="57" customHeight="1">
+    <row r="31" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="s">
         <v>54</v>
       </c>
@@ -2058,7 +2069,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="60">
+    <row r="33" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
         <v>22</v>
       </c>
@@ -2084,7 +2095,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="20"/>
       <c r="B34" s="15"/>
       <c r="C34" s="21"/>
@@ -2094,7 +2105,7 @@
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
     </row>
-    <row r="35" spans="1:8" ht="60">
+    <row r="35" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
         <v>125</v>
       </c>
@@ -2120,7 +2131,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="15.6" customHeight="1">
+    <row r="36" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="20"/>
       <c r="B36" s="15"/>
       <c r="C36" s="21"/>
@@ -2130,7 +2141,7 @@
       <c r="G36" s="15"/>
       <c r="H36" s="15"/>
     </row>
-    <row r="37" spans="1:8" ht="61.9" customHeight="1">
+    <row r="37" spans="1:8" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
         <v>131</v>
       </c>
@@ -2156,7 +2167,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="15" customHeight="1">
+    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="20"/>
       <c r="B38" s="15"/>
       <c r="C38" s="21"/>
@@ -2166,7 +2177,7 @@
       <c r="G38" s="15"/>
       <c r="H38" s="15"/>
     </row>
-    <row r="39" spans="1:8" ht="45">
+    <row r="39" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="20" t="s">
         <v>157</v>
       </c>
@@ -2192,7 +2203,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="17.45" customHeight="1">
+    <row r="40" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="20"/>
       <c r="B40" s="15"/>
       <c r="C40" s="21"/>
@@ -2202,7 +2213,7 @@
       <c r="G40" s="15"/>
       <c r="H40" s="15"/>
     </row>
-    <row r="41" spans="1:8" ht="64.150000000000006" customHeight="1">
+    <row r="41" spans="1:8" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
         <v>202</v>
       </c>
@@ -2228,7 +2239,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="17.45" customHeight="1">
+    <row r="42" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="20"/>
       <c r="B42" s="15"/>
       <c r="C42" s="21"/>
@@ -2238,7 +2249,7 @@
       <c r="G42" s="15"/>
       <c r="H42" s="15"/>
     </row>
-    <row r="43" spans="1:8" ht="60">
+    <row r="43" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A43" s="20" t="s">
         <v>48</v>
       </c>
@@ -2264,7 +2275,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="20"/>
       <c r="B44" s="15"/>
       <c r="C44" s="21"/>
@@ -2274,7 +2285,7 @@
       <c r="G44" s="15"/>
       <c r="H44" s="15"/>
     </row>
-    <row r="45" spans="1:8" ht="60">
+    <row r="45" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" s="20" t="s">
         <v>54</v>
       </c>
@@ -2300,7 +2311,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="20"/>
       <c r="B46" s="15"/>
       <c r="C46" s="21"/>
@@ -2310,7 +2321,7 @@
       <c r="G46" s="15"/>
       <c r="H46" s="15"/>
     </row>
-    <row r="47" spans="1:8" ht="45">
+    <row r="47" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A47" s="20" t="s">
         <v>129</v>
       </c>
@@ -2336,7 +2347,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="20"/>
       <c r="B48" s="15"/>
       <c r="C48" s="21"/>
@@ -2346,7 +2357,7 @@
       <c r="G48" s="15"/>
       <c r="H48" s="15"/>
     </row>
-    <row r="49" spans="1:8" ht="60">
+    <row r="49" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A49" s="20" t="s">
         <v>49</v>
       </c>
@@ -2372,7 +2383,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="20"/>
       <c r="B50" s="15"/>
       <c r="C50" s="21"/>
@@ -2382,7 +2393,7 @@
       <c r="G50" s="15"/>
       <c r="H50" s="15"/>
     </row>
-    <row r="51" spans="1:8" ht="60">
+    <row r="51" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A51" s="20" t="s">
         <v>109</v>
       </c>
@@ -2408,7 +2419,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="20"/>
       <c r="B52" s="15"/>
       <c r="C52" s="21"/>
@@ -2418,7 +2429,7 @@
       <c r="G52" s="15"/>
       <c r="H52" s="15"/>
     </row>
-    <row r="53" spans="1:8" ht="60">
+    <row r="53" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A53" s="20" t="s">
         <v>111</v>
       </c>
@@ -2444,7 +2455,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="20"/>
       <c r="B54" s="15"/>
       <c r="C54" s="21"/>
@@ -2454,7 +2465,7 @@
       <c r="G54" s="15"/>
       <c r="H54" s="15"/>
     </row>
-    <row r="55" spans="1:8" ht="58.15" customHeight="1">
+    <row r="55" spans="1:8" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="20" t="s">
         <v>119</v>
       </c>
@@ -2480,9 +2491,11 @@
         <v>228</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="20"/>
-      <c r="B56" s="15"/>
+      <c r="B56" s="15" t="s">
+        <v>287</v>
+      </c>
       <c r="C56" s="21"/>
       <c r="D56" s="20"/>
       <c r="E56" s="20"/>
@@ -2495,22 +2508,22 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task status" prompt="Current status of task. One of: Planned, In Progress, On Hold, Completed" sqref="F57:F1048576 F4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task status" prompt="Current status of task. One of: Planned, In Progress, On Hold, Completed" sqref="F57:F1048576 F4" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Planned, In Progress, On Hold, Completed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Priority" prompt="Priority of task. One of: Critical, High, Medium, Low" sqref="E57:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Priority" prompt="Priority of task. One of: Critical, High, Medium, Low" sqref="E57:E1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Critical, High, Medium, Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Story. One of: Planned, In Progress, On Hold, Completed" sqref="F6:F31 F33:F56">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Story. One of: Planned, In Progress, On Hold, Completed" sqref="F6:F31 F33:F56" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Not in sprint, Sprint 1, Sprint 2, Sprint 3, In Progress, On Hold, Completed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E6:E31 E33:E56">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E6:E31 E33:E56" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"Sprint 1, Sprint 2, Sprint 3, Future"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Is the task completed?" prompt="Describe the criteria to be used to determine if the task is completed as per requirements.&#10;" sqref="H5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Card. One of: Planned, In Progress, On Hold, Completed" sqref="F5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Story Point" prompt="Story point is an arbitary measure used to measure the effort required to implement a story.&#10;&#10;" sqref="D5"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Is the task completed?" prompt="Describe the criteria to be used to determine if the task is completed as per requirements._x000a_" sqref="H5" xr:uid="{00000000-0002-0000-0100-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E5" xr:uid="{00000000-0002-0000-0100-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Card. One of: Planned, In Progress, On Hold, Completed" sqref="F5" xr:uid="{00000000-0002-0000-0100-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Story Point" prompt="Story point is an arbitary measure used to measure the effort required to implement a story._x000a__x000a_" sqref="D5" xr:uid="{00000000-0002-0000-0100-000007000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="60" orientation="landscape" r:id="rId1"/>
@@ -2518,7 +2531,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2528,16 +2541,16 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="25.140625" customWidth="1"/>
-    <col min="4" max="4" width="44.42578125" customWidth="1"/>
-    <col min="5" max="6" width="7.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="43.140625" customWidth="1"/>
+    <col min="3" max="3" width="25.109375" customWidth="1"/>
+    <col min="4" max="4" width="44.44140625" customWidth="1"/>
+    <col min="5" max="6" width="7.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" customWidth="1"/>
+    <col min="8" max="8" width="43.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>5</v>
       </c>
@@ -2549,7 +2562,7 @@
       <c r="G1" s="26"/>
       <c r="H1" s="26"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
         <v>265</v>
       </c>
@@ -2560,7 +2573,7 @@
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="28" t="s">
         <v>83</v>
       </c>
@@ -2570,7 +2583,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="6" customFormat="1" ht="40.5" customHeight="1">
+    <row r="6" spans="1:8" s="6" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
@@ -2594,7 +2607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="135">
+    <row r="7" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -2620,7 +2633,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="60">
+    <row r="8" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -2646,7 +2659,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="60">
+    <row r="9" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
@@ -2672,7 +2685,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="60">
+    <row r="10" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -2698,7 +2711,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="60">
+    <row r="11" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
@@ -2724,7 +2737,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="75">
+    <row r="12" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
@@ -2750,7 +2763,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="45">
+    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>30</v>
       </c>
@@ -2776,7 +2789,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="60">
+    <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
@@ -2802,7 +2815,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="75">
+    <row r="15" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>30</v>
       </c>
@@ -2828,7 +2841,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="45">
+    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
@@ -2854,7 +2867,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="60">
+    <row r="17" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
@@ -2880,7 +2893,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="45">
+    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>29</v>
       </c>
@@ -2906,7 +2919,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="45">
+    <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>29</v>
       </c>
@@ -2932,7 +2945,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="45">
+    <row r="20" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>29</v>
       </c>
@@ -2958,7 +2971,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="45">
+    <row r="21" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>43</v>
       </c>
@@ -2984,7 +2997,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="60">
+    <row r="22" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>43</v>
       </c>
@@ -3010,7 +3023,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="30">
+    <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>43</v>
       </c>
@@ -3036,7 +3049,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="45">
+    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>104</v>
       </c>
@@ -3069,9 +3082,9 @@
     <mergeCell ref="A5:B5"/>
   </mergeCells>
   <dataValidations xWindow="1022" yWindow="574" count="3">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G6"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimate" prompt="Estimated hours for the task." sqref="E6:F6"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G7:G20 G21:G24">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G6" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimate" prompt="Estimated hours for the task." sqref="E6:F6" xr:uid="{00000000-0002-0000-0200-000001000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G7:G20 G21:G24" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>"Planned, In Progress, On Hold, Completed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3081,24 +3094,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" customWidth="1"/>
+    <col min="4" max="4" width="25.44140625" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>118</v>
       </c>
@@ -3110,7 +3123,7 @@
       <c r="G1" s="26"/>
       <c r="H1" s="26"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>286</v>
       </c>
@@ -3122,7 +3135,7 @@
       <c r="G4" s="29"/>
       <c r="H4" s="29"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="28" t="s">
         <v>83</v>
       </c>
@@ -3132,7 +3145,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30">
+    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
@@ -3156,7 +3169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="60">
+    <row r="7" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>169</v>
       </c>
@@ -3182,7 +3195,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="60">
+    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>50</v>
       </c>
@@ -3208,7 +3221,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30">
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
@@ -3234,7 +3247,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="45">
+    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -3260,7 +3273,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="45">
+    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
@@ -3286,7 +3299,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30">
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -3312,7 +3325,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="60">
+    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
@@ -3338,7 +3351,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30">
+    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>147</v>
       </c>
@@ -3364,7 +3377,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="60">
+    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>169</v>
       </c>
@@ -3390,7 +3403,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="45">
+    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>157</v>
       </c>
@@ -3416,7 +3429,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="45">
+    <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>202</v>
       </c>
@@ -3442,7 +3455,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="60">
+    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>147</v>
       </c>
@@ -3468,7 +3481,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="45">
+    <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>147</v>
       </c>
@@ -3494,7 +3507,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="60">
+    <row r="20" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>169</v>
       </c>
@@ -3520,7 +3533,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="60">
+    <row r="21" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>27</v>
       </c>
@@ -3546,7 +3559,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="87" customHeight="1">
+    <row r="22" spans="1:8" ht="87" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>125</v>
       </c>
@@ -3572,7 +3585,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="60">
+    <row r="23" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>125</v>
       </c>
@@ -3598,7 +3611,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="30.75" customHeight="1">
+    <row r="24" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>43</v>
       </c>
@@ -3624,7 +3637,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="45" customHeight="1">
+    <row r="25" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>43</v>
       </c>
@@ -3650,7 +3663,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="45">
+    <row r="26" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>131</v>
       </c>
@@ -3676,7 +3689,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="45">
+    <row r="27" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>180</v>
       </c>
@@ -3702,7 +3715,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="30">
+    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>156</v>
       </c>
@@ -3728,7 +3741,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="60">
+    <row r="29" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>157</v>
       </c>
@@ -3754,7 +3767,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="45">
+    <row r="30" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>182</v>
       </c>
@@ -3780,7 +3793,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="30">
+    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>183</v>
       </c>
@@ -3811,11 +3824,11 @@
     <mergeCell ref="A4:H4"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G7:G31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G7:G31" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Planned, In Progress, On Hold, Completed"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimate" prompt="Estimated hours for the task." sqref="E6:F6"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G6"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimate" prompt="Estimated hours for the task." sqref="E6:F6" xr:uid="{00000000-0002-0000-0300-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G6" xr:uid="{00000000-0002-0000-0300-000002000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3823,12 +3836,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Preparations fro Sprint 3
-Added tasks in product Backlog from sprint 2
-Moved unfinished tasks in Sprint 2 to Sprint 3 (Product Backlog)
</commit_message>
<xml_diff>
--- a/Documentation/Product Backlog.xlsx
+++ b/Documentation/Product Backlog.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22215"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomil\StudioProjects\ELEC-COEN-390\Documentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CAE12F1-7AAC-40DF-A3E9-D0FBF1A13BD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="5" r:id="rId1"/>
@@ -19,9 +13,10 @@
     <sheet name="Sprint 2" sheetId="3" r:id="rId4"/>
     <sheet name="Sprint 3" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="291">
   <si>
     <t>Story ID</t>
   </si>
@@ -142,12 +137,6 @@
   </si>
   <si>
     <t>The presenter will be able unlock the door and open it.</t>
-  </si>
-  <si>
-    <t>The presenter is sure that the door is always locked unless opened by them.</t>
-  </si>
-  <si>
-    <t>Default State Locked</t>
   </si>
   <si>
     <t>Unlock Door</t>
@@ -428,12 +417,6 @@
 • Password is stored in the database</t>
   </si>
   <si>
-    <t>Add Doors to Profile</t>
-  </si>
-  <si>
-    <t>BE-7</t>
-  </si>
-  <si>
     <t>• Be able to peek and unlock multiple doors</t>
   </si>
   <si>
@@ -447,9 +430,6 @@
   </si>
   <si>
     <t>• Confirmation from the stakeholders</t>
-  </si>
-  <si>
-    <t>Connect Arduino Wifi</t>
   </si>
   <si>
     <t>Connect Arduino Database</t>
@@ -658,13 +638,6 @@
     <t>As an administrator, I want the app to scan the picture of me it took at the door so that it verifies that I am an admin and unlock the door automatically for me. (Epic)</t>
   </si>
   <si>
-    <t>The application should allow users to prevent others from unlocking a door.</t>
-  </si>
-  <si>
-    <t>• Deleting a user removes them from the database
-• Requires them to Sign Up again</t>
-  </si>
-  <si>
     <t>The user should be able to add additionnal doors to the appliaction, in order to access them by deleting other in Administrators page.</t>
   </si>
   <si>
@@ -713,12 +686,6 @@
     <t>As an user, I want be able to modify values in my profile to represent my present reality. (Story)</t>
   </si>
   <si>
-    <t>As an user, I want to be able to control multiple doors through the application to minimize the amount of time I need to log in and log out. (Story)</t>
-  </si>
-  <si>
-    <t>As a presenter, I want the make sure the door is always locked whenever I choose to not open it to ensure security. (Story)</t>
-  </si>
-  <si>
     <t>As a presenter, I want the ability to select the Open Door button to access the door without being physically there to save time and energy. (Epic)</t>
   </si>
   <si>
@@ -726,9 +693,6 @@
   </si>
   <si>
     <t>As an administrator, I want the the history page to also record the user's device that open the door so that I can monitor which administrators opens the door (Epic)</t>
-  </si>
-  <si>
-    <t>The app shows which administrator has opened the door. (Epic)</t>
   </si>
   <si>
     <t>• The history page shows the admin who opened the door along with the user that was at the door</t>
@@ -957,12 +921,51 @@
   <si>
     <t>RFID</t>
   </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>The app shows which administrator has opened the door.</t>
+  </si>
+  <si>
+    <t>Rasberry -Pi Holder</t>
+  </si>
+  <si>
+    <t>Connect Rasberry -Pi Wifi</t>
+  </si>
+  <si>
+    <t>Refactor Display History</t>
+  </si>
+  <si>
+    <t>GEN-11</t>
+  </si>
+  <si>
+    <t>GEN-12</t>
+  </si>
+  <si>
+    <t>As an user, I want be able to view the history of people who attempted to open the door in descending chronological order to know who was a the door. (Story)</t>
+  </si>
+  <si>
+    <t>The user should be viwing images taken by the camera in descending orer chronologically, only the Firebase strorage should be used.</t>
+  </si>
+  <si>
+    <t>• Be to retrieve images from the storage in descending order of date without using Cloud Firestore</t>
+  </si>
+  <si>
+    <t>As a .user, I want the ability to unlock my door even when there is no internet connection to be able to open my door during extreme weather conditions.</t>
+  </si>
+  <si>
+    <t>The RFID should allow the user to unlock the door without using the Android application.</t>
+  </si>
+  <si>
+    <t>• Unlock the door using RFID</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1434,89 +1437,89 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="126.6640625" customWidth="1"/>
+    <col min="1" max="1" width="126.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="7" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:1" s="7" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" s="7" customFormat="1" ht="13.5" customHeight="1"/>
+    <row r="2" spans="1:1" s="7" customFormat="1"/>
+    <row r="3" spans="1:1" s="7" customFormat="1" ht="26.25">
       <c r="A3" s="8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:1" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" s="7" customFormat="1"/>
+    <row r="5" spans="1:1" s="7" customFormat="1"/>
+    <row r="6" spans="1:1" s="7" customFormat="1" ht="21">
       <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" s="7" customFormat="1">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:1" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:1" s="7" customFormat="1" ht="21">
       <c r="A8" s="9" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:1" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" s="7" customFormat="1"/>
+    <row r="10" spans="1:1" s="11" customFormat="1" ht="18.75">
       <c r="A10" s="10" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" s="11" customFormat="1" ht="18.75">
       <c r="A11" s="10" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" s="11" customFormat="1" ht="18.75">
       <c r="A12" s="10" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" s="7" customFormat="1" ht="18.75">
       <c r="A13" s="10" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" s="7" customFormat="1" ht="18.75">
       <c r="A14" s="10" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="17" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="18" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="19" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="20" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="21" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="22" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="23" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="24" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="25" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="26" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="27" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="28" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="29" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="30" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" s="7" customFormat="1"/>
+    <row r="16" spans="1:1" s="7" customFormat="1"/>
+    <row r="17" s="7" customFormat="1"/>
+    <row r="18" s="7" customFormat="1"/>
+    <row r="19" s="7" customFormat="1"/>
+    <row r="20" s="7" customFormat="1"/>
+    <row r="21" s="7" customFormat="1"/>
+    <row r="22" s="7" customFormat="1"/>
+    <row r="23" s="7" customFormat="1"/>
+    <row r="24" s="7" customFormat="1"/>
+    <row r="25" s="7" customFormat="1"/>
+    <row r="26" s="7" customFormat="1"/>
+    <row r="27" s="7" customFormat="1"/>
+    <row r="28" s="7" customFormat="1"/>
+    <row r="29" s="7" customFormat="1"/>
+    <row r="30" s="7" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -1524,30 +1527,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="16"/>
-    <col min="2" max="2" width="18.44140625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="44.44140625" style="16" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="16" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="16" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" style="16" customWidth="1"/>
-    <col min="7" max="7" width="46.6640625" style="16" customWidth="1"/>
-    <col min="8" max="8" width="42.5546875" style="16" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="16"/>
+    <col min="1" max="1" width="8.85546875" style="16"/>
+    <col min="2" max="2" width="18.42578125" style="16" customWidth="1"/>
+    <col min="3" max="3" width="44.42578125" style="16" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="16" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="16" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="46.7109375" style="16" customWidth="1"/>
+    <col min="8" max="8" width="42.5703125" style="16" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="21">
       <c r="A1" s="24" t="s">
         <v>4</v>
       </c>
@@ -1559,7 +1562,7 @@
       <c r="G1" s="25"/>
       <c r="H1" s="25"/>
     </row>
-    <row r="5" spans="1:8" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="23" customFormat="1" ht="40.5" customHeight="1">
       <c r="A5" s="22" t="s">
         <v>0</v>
       </c>
@@ -1570,7 +1573,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>7</v>
@@ -1585,7 +1588,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="120">
       <c r="A6" s="17" t="s">
         <v>17</v>
       </c>
@@ -1602,16 +1605,16 @@
         <v>16</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="20"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
@@ -1621,7 +1624,7 @@
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
     </row>
-    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="60">
       <c r="A8" s="17" t="s">
         <v>20</v>
       </c>
@@ -1638,16 +1641,16 @@
         <v>16</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G8" s="18" t="s">
         <v>31</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="20"/>
       <c r="B9" s="15"/>
       <c r="C9" s="21"/>
@@ -1657,15 +1660,15 @@
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
     </row>
-    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="30">
       <c r="A10" s="20" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="D10" s="20">
         <v>3</v>
@@ -1674,16 +1677,16 @@
         <v>16</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="20"/>
       <c r="B11" s="15"/>
       <c r="C11" s="21"/>
@@ -1693,15 +1696,15 @@
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
     </row>
-    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="45">
       <c r="A12" s="20" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="D12" s="20">
         <v>3</v>
@@ -1710,24 +1713,24 @@
         <v>16</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="45">
       <c r="A13" s="20" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="D13" s="20">
         <v>5</v>
@@ -1736,16 +1739,16 @@
         <v>16</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="20"/>
       <c r="B14" s="15"/>
       <c r="C14" s="21"/>
@@ -1755,15 +1758,15 @@
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
     </row>
-    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="45">
       <c r="A15" s="20" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D15" s="20">
         <v>3</v>
@@ -1772,16 +1775,16 @@
         <v>16</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="20"/>
       <c r="B16" s="15"/>
       <c r="C16" s="21"/>
@@ -1791,33 +1794,33 @@
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
     </row>
-    <row r="17" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="45">
       <c r="A17" s="20" t="s">
-        <v>144</v>
+        <v>29</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>145</v>
+        <v>26</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>214</v>
+        <v>57</v>
       </c>
       <c r="D17" s="20">
         <v>3</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>146</v>
+        <v>36</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="20"/>
       <c r="B18" s="15"/>
       <c r="C18" s="21"/>
@@ -1827,33 +1830,33 @@
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
     </row>
-    <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="75">
       <c r="A19" s="20" t="s">
-        <v>147</v>
+        <v>27</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>148</v>
+        <v>251</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>215</v>
+        <v>253</v>
       </c>
       <c r="D19" s="20">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.6" customHeight="1">
       <c r="A20" s="20"/>
       <c r="B20" s="15"/>
       <c r="C20" s="21"/>
@@ -1863,33 +1866,33 @@
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
     </row>
-    <row r="21" spans="1:8" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="20" t="s">
-        <v>156</v>
+    <row r="21" spans="1:8" ht="56.45" customHeight="1">
+      <c r="A21" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>143</v>
+        <v>71</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="D21" s="20">
-        <v>3</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>123</v>
+        <v>209</v>
+      </c>
+      <c r="D21" s="15">
+        <v>5</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>121</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="19.149999999999999" customHeight="1">
       <c r="A22" s="20"/>
       <c r="B22" s="15"/>
       <c r="C22" s="21"/>
@@ -1899,69 +1902,60 @@
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
     </row>
-    <row r="23" spans="1:8" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="61.9" customHeight="1">
       <c r="A23" s="20" t="s">
-        <v>157</v>
+        <v>52</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>141</v>
+        <v>35</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>158</v>
+        <v>101</v>
       </c>
       <c r="D23" s="20">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G23" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="17.45" customHeight="1"/>
+    <row r="25" spans="1:8" ht="56.45" customHeight="1">
+      <c r="A25" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="H23" s="15" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="20"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-    </row>
-    <row r="25" spans="1:8" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>26</v>
-      </c>
       <c r="C25" s="21" t="s">
-        <v>59</v>
+        <v>211</v>
       </c>
       <c r="D25" s="20">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="20"/>
       <c r="B26" s="15"/>
       <c r="C26" s="21"/>
@@ -1971,33 +1965,33 @@
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
     </row>
-    <row r="27" spans="1:8" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="56.45" customHeight="1">
       <c r="A27" s="20" t="s">
-        <v>27</v>
+        <v>197</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>261</v>
+        <v>200</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>263</v>
+        <v>214</v>
       </c>
       <c r="D27" s="20">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>87</v>
+        <v>202</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="20"/>
       <c r="B28" s="15"/>
       <c r="C28" s="21"/>
@@ -2007,33 +2001,33 @@
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
     </row>
-    <row r="29" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="15" t="s">
-        <v>43</v>
+    <row r="29" spans="1:8" ht="60">
+      <c r="A29" s="20" t="s">
+        <v>46</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>73</v>
+        <v>173</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>216</v>
-      </c>
-      <c r="D29" s="15">
-        <v>5</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="F29" s="15" t="s">
-        <v>123</v>
+        <v>210</v>
+      </c>
+      <c r="D29" s="20">
+        <v>3</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="F29" s="20" t="s">
+        <v>121</v>
       </c>
       <c r="G29" s="15" t="s">
-        <v>74</v>
+        <v>174</v>
       </c>
       <c r="H29" s="15" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="21" customHeight="1">
       <c r="A30" s="20"/>
       <c r="B30" s="15"/>
       <c r="C30" s="21"/>
@@ -2043,59 +2037,69 @@
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>
     </row>
-    <row r="31" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="57" customHeight="1">
       <c r="A31" s="20" t="s">
-        <v>54</v>
+        <v>283</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>37</v>
+        <v>282</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>103</v>
+        <v>285</v>
       </c>
       <c r="D31" s="20">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>34</v>
+        <v>286</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="20"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+    </row>
+    <row r="33" spans="1:8" ht="60">
       <c r="A33" s="20" t="s">
-        <v>22</v>
+        <v>284</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>40</v>
+        <v>277</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>218</v>
+        <v>288</v>
       </c>
       <c r="D33" s="20">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>33</v>
+        <v>289</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="20"/>
       <c r="B34" s="15"/>
       <c r="C34" s="21"/>
@@ -2105,33 +2109,33 @@
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
     </row>
-    <row r="35" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="60">
       <c r="A35" s="20" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="D35" s="20">
         <v>5</v>
       </c>
       <c r="E35" s="20" t="s">
-        <v>123</v>
+        <v>278</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>123</v>
+        <v>278</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.6" customHeight="1">
       <c r="A36" s="20"/>
       <c r="B36" s="15"/>
       <c r="C36" s="21"/>
@@ -2141,33 +2145,33 @@
       <c r="G36" s="15"/>
       <c r="H36" s="15"/>
     </row>
-    <row r="37" spans="1:8" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="61.9" customHeight="1">
       <c r="A37" s="20" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="D37" s="20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>123</v>
+        <v>278</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>123</v>
+        <v>278</v>
       </c>
       <c r="G37" s="15" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="H37" s="15" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15" customHeight="1">
       <c r="A38" s="20"/>
       <c r="B38" s="15"/>
       <c r="C38" s="21"/>
@@ -2177,33 +2181,33 @@
       <c r="G38" s="15"/>
       <c r="H38" s="15"/>
     </row>
-    <row r="39" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="45">
       <c r="A39" s="20" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>201</v>
+        <v>143</v>
       </c>
       <c r="C39" s="21" t="s">
         <v>208</v>
       </c>
       <c r="D39" s="20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E39" s="20" t="s">
-        <v>123</v>
+        <v>278</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>123</v>
+        <v>278</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>206</v>
+        <v>144</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="17.45" customHeight="1">
       <c r="A40" s="20"/>
       <c r="B40" s="15"/>
       <c r="C40" s="21"/>
@@ -2213,33 +2217,33 @@
       <c r="G40" s="15"/>
       <c r="H40" s="15"/>
     </row>
-    <row r="41" spans="1:8" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="64.150000000000006" customHeight="1">
       <c r="A41" s="20" t="s">
-        <v>202</v>
+        <v>151</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>207</v>
+        <v>138</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>221</v>
+        <v>147</v>
       </c>
       <c r="D41" s="20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E41" s="20" t="s">
-        <v>123</v>
+        <v>278</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>123</v>
+        <v>278</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>209</v>
+        <v>36</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="17.45" customHeight="1">
       <c r="A42" s="20"/>
       <c r="B42" s="15"/>
       <c r="C42" s="21"/>
@@ -2249,33 +2253,33 @@
       <c r="G42" s="15"/>
       <c r="H42" s="15"/>
     </row>
-    <row r="43" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" ht="45">
       <c r="A43" s="20" t="s">
-        <v>48</v>
+        <v>152</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>178</v>
+        <v>280</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>217</v>
+        <v>153</v>
       </c>
       <c r="D43" s="20">
         <v>3</v>
       </c>
       <c r="E43" s="20" t="s">
-        <v>123</v>
+        <v>278</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>123</v>
+        <v>278</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>179</v>
+        <v>36</v>
       </c>
       <c r="H43" s="15" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" s="20"/>
       <c r="B44" s="15"/>
       <c r="C44" s="21"/>
@@ -2285,33 +2289,33 @@
       <c r="G44" s="15"/>
       <c r="H44" s="15"/>
     </row>
-    <row r="45" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="45">
       <c r="A45" s="20" t="s">
-        <v>54</v>
+        <v>127</v>
       </c>
       <c r="B45" s="15" t="s">
         <v>128</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="D45" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E45" s="20" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F45" s="20" t="s">
-        <v>112</v>
+        <v>278</v>
       </c>
       <c r="G45" s="15" t="s">
-        <v>204</v>
+        <v>129</v>
       </c>
       <c r="H45" s="15" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" s="20"/>
       <c r="B46" s="15"/>
       <c r="C46" s="21"/>
@@ -2321,33 +2325,33 @@
       <c r="G46" s="15"/>
       <c r="H46" s="15"/>
     </row>
-    <row r="47" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" ht="45">
       <c r="A47" s="20" t="s">
-        <v>129</v>
+        <v>152</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>36</v>
+        <v>196</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>223</v>
+        <v>201</v>
       </c>
       <c r="D47" s="20">
         <v>2</v>
       </c>
       <c r="E47" s="20" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>112</v>
+        <v>278</v>
       </c>
       <c r="G47" s="15" t="s">
-        <v>35</v>
+        <v>199</v>
       </c>
       <c r="H47" s="15" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" s="20"/>
       <c r="B48" s="15"/>
       <c r="C48" s="21"/>
@@ -2357,33 +2361,33 @@
       <c r="G48" s="15"/>
       <c r="H48" s="15"/>
     </row>
-    <row r="49" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" ht="60">
       <c r="A49" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="D49" s="20">
         <v>3</v>
       </c>
       <c r="E49" s="20" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F49" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G49" s="15" t="s">
         <v>32</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" s="20"/>
       <c r="B50" s="15"/>
       <c r="C50" s="21"/>
@@ -2393,33 +2397,33 @@
       <c r="G50" s="15"/>
       <c r="H50" s="15"/>
     </row>
-    <row r="51" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" ht="60">
       <c r="A51" s="20" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D51" s="20">
         <v>13</v>
       </c>
       <c r="E51" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="F51" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="G51" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="F51" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="G51" s="15" t="s">
-        <v>117</v>
-      </c>
       <c r="H51" s="15" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" s="20"/>
       <c r="B52" s="15"/>
       <c r="C52" s="21"/>
@@ -2429,33 +2433,33 @@
       <c r="G52" s="15"/>
       <c r="H52" s="15"/>
     </row>
-    <row r="53" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" ht="60">
       <c r="A53" s="20" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D53" s="20">
         <v>21</v>
       </c>
       <c r="E53" s="20" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F53" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G53" s="15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H53" s="15" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54" s="20"/>
       <c r="B54" s="15"/>
       <c r="C54" s="21"/>
@@ -2465,37 +2469,35 @@
       <c r="G54" s="15"/>
       <c r="H54" s="15"/>
     </row>
-    <row r="55" spans="1:8" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" ht="58.15" customHeight="1">
       <c r="A55" s="20" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C55" s="21" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="D55" s="20">
         <v>3</v>
       </c>
       <c r="E55" s="20" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F55" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G55" s="15" t="s">
-        <v>227</v>
+        <v>279</v>
       </c>
       <c r="H55" s="15" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56" s="20"/>
-      <c r="B56" s="15" t="s">
-        <v>287</v>
-      </c>
+      <c r="B56" s="15"/>
       <c r="C56" s="21"/>
       <c r="D56" s="20"/>
       <c r="E56" s="20"/>
@@ -2507,23 +2509,23 @@
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
-  <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task status" prompt="Current status of task. One of: Planned, In Progress, On Hold, Completed" sqref="F57:F1048576 F4" xr:uid="{00000000-0002-0000-0100-000000000000}">
+  <dataValidations xWindow="650" yWindow="542" count="8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task status" prompt="Current status of task. One of: Planned, In Progress, On Hold, Completed" sqref="F57:F1048576 F4">
       <formula1>"Planned, In Progress, On Hold, Completed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Priority" prompt="Priority of task. One of: Critical, High, Medium, Low" sqref="E57:E1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Priority" prompt="Priority of task. One of: Critical, High, Medium, Low" sqref="E57:E1048576">
       <formula1>"Critical, High, Medium, Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Story. One of: Planned, In Progress, On Hold, Completed" sqref="F6:F31 F33:F56" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Story. One of: Planned, In Progress, On Hold, Completed" sqref="F6:F23 F25:F56">
       <formula1>"Not in sprint, Sprint 1, Sprint 2, Sprint 3, In Progress, On Hold, Completed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E6:E31 E33:E56" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E6:E23 E25:E56">
       <formula1>"Sprint 1, Sprint 2, Sprint 3, Future"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Is the task completed?" prompt="Describe the criteria to be used to determine if the task is completed as per requirements._x000a_" sqref="H5" xr:uid="{00000000-0002-0000-0100-000004000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E5" xr:uid="{00000000-0002-0000-0100-000005000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Card. One of: Planned, In Progress, On Hold, Completed" sqref="F5" xr:uid="{00000000-0002-0000-0100-000006000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Story Point" prompt="Story point is an arbitary measure used to measure the effort required to implement a story._x000a__x000a_" sqref="D5" xr:uid="{00000000-0002-0000-0100-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Is the task completed?" prompt="Describe the criteria to be used to determine if the task is completed as per requirements.&#10;" sqref="H5"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E5"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Card. One of: Planned, In Progress, On Hold, Completed" sqref="F5"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Story Point" prompt="Story point is an arbitary measure used to measure the effort required to implement a story.&#10;&#10;" sqref="D5"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="60" orientation="landscape" r:id="rId1"/>
@@ -2531,7 +2533,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2541,16 +2543,16 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="25.109375" customWidth="1"/>
-    <col min="4" max="4" width="44.44140625" customWidth="1"/>
-    <col min="5" max="6" width="7.44140625" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" customWidth="1"/>
-    <col min="8" max="8" width="43.109375" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="44.42578125" customWidth="1"/>
+    <col min="5" max="6" width="7.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="21">
       <c r="A1" s="26" t="s">
         <v>5</v>
       </c>
@@ -2562,9 +2564,9 @@
       <c r="G1" s="26"/>
       <c r="H1" s="26"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" s="27" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="B4" s="27"/>
       <c r="C4" s="27"/>
@@ -2573,9 +2575,9 @@
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" s="28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B5" s="28"/>
       <c r="C5">
@@ -2583,7 +2585,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="6" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="6" customFormat="1" ht="40.5" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
@@ -2607,7 +2609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="135">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -2615,25 +2617,25 @@
         <v>17</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E7" s="2">
         <v>2</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="60">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -2650,42 +2652,42 @@
         <v>2</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="60">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E9" s="3">
         <v>5</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="60">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -2693,386 +2695,386 @@
         <v>25</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E10" s="3">
         <v>3</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="60">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E11" s="3">
         <v>5</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="75">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E12" s="3">
         <v>1</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="45">
       <c r="A13" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="13" t="s">
         <v>68</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>70</v>
       </c>
       <c r="E13" s="2">
         <v>5</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="60">
       <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E14" s="2">
         <v>5</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="75">
       <c r="A15" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E15" s="2">
         <v>5</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="45">
       <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E16" s="2">
         <v>5</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="60">
       <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E17" s="2">
         <v>5</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="45">
       <c r="A18" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E18" s="2">
         <v>5</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="45">
       <c r="A19" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E19" s="2">
         <v>5</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="45">
       <c r="A20" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E20" s="2">
         <v>5</v>
       </c>
       <c r="F20" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="45">
+      <c r="A21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="13" t="s">
         <v>80</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>82</v>
       </c>
       <c r="E21" s="2">
         <v>5</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="60">
       <c r="A22" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E22" s="2">
         <v>5</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="30">
       <c r="A23" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="E23" s="2">
         <v>5</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="45">
       <c r="A24" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="D24" s="13" t="s">
         <v>104</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>106</v>
       </c>
       <c r="E24" s="2">
         <v>5</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -3082,9 +3084,9 @@
     <mergeCell ref="A5:B5"/>
   </mergeCells>
   <dataValidations xWindow="1022" yWindow="574" count="3">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G6" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimate" prompt="Estimated hours for the task." sqref="E6:F6" xr:uid="{00000000-0002-0000-0200-000001000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G7:G20 G21:G24" xr:uid="{00000000-0002-0000-0200-000002000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G6"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimate" prompt="Estimated hours for the task." sqref="E6:F6"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G7:G20 G21:G24">
       <formula1>"Planned, In Progress, On Hold, Completed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3094,26 +3096,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="21.109375" customWidth="1"/>
-    <col min="4" max="4" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="21">
       <c r="A1" s="26" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -3123,9 +3125,9 @@
       <c r="G1" s="26"/>
       <c r="H1" s="26"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" s="29" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="B4" s="29"/>
       <c r="C4" s="29"/>
@@ -3135,9 +3137,9 @@
       <c r="G4" s="29"/>
       <c r="H4" s="29"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" s="28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B5" s="28"/>
       <c r="C5">
@@ -3145,7 +3147,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="30">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
@@ -3169,41 +3171,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="60">
       <c r="A7" s="3" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>135</v>
+        <v>281</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E7" s="3">
         <v>5</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="60">
       <c r="A8" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>33</v>
@@ -3212,328 +3214,328 @@
         <v>5</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E9" s="2">
         <v>2</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="45">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E10" s="2">
         <v>3</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="45">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="E11" s="2">
         <v>3</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E12" s="2">
         <v>2</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="60">
       <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E13" s="2">
         <v>3</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30">
       <c r="A14" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E14" s="2">
         <v>2</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="60">
       <c r="A15" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E15" s="2">
         <v>5</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="45">
       <c r="A16" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="E16" s="2">
         <v>4</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="45">
       <c r="A17" s="2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="E17" s="2">
         <v>4</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="60">
       <c r="A18" s="3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E18" s="3">
         <v>5</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="45">
       <c r="A19" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E19" s="2">
         <v>3</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="60">
       <c r="A20" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E20" s="3">
         <v>5</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="60">
       <c r="A21" s="2" t="s">
         <v>27</v>
       </c>
@@ -3541,276 +3543,276 @@
         <v>27</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="E21" s="2">
         <v>5</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="87" customHeight="1" x14ac:dyDescent="0.3">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="87" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="E22" s="2">
         <v>5</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="60">
       <c r="A23" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E23" s="2">
         <v>5</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="30.75" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E24" s="2">
         <v>5</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="45" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E25" s="3">
         <v>5</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="45">
       <c r="A26" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E26" s="2">
         <v>3</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="45">
       <c r="A27" s="2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E27" s="2">
         <v>5</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="30">
       <c r="A28" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E28" s="2">
         <v>2</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="60">
       <c r="A29" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E29" s="2">
         <v>4</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="45">
       <c r="A30" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E30" s="2">
         <v>4</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="30">
       <c r="A31" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E31" s="2">
         <v>3</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>15</v>
@@ -3824,11 +3826,11 @@
     <mergeCell ref="A4:H4"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G7:G31" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G7:G31">
       <formula1>"Planned, In Progress, On Hold, Completed"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimate" prompt="Estimated hours for the task." sqref="E6:F6" xr:uid="{00000000-0002-0000-0300-000001000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G6" xr:uid="{00000000-0002-0000-0300-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimate" prompt="Estimated hours for the task." sqref="E6:F6"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G6"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3836,12 +3838,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Grooming Product Backlog for Sprint 3
</commit_message>
<xml_diff>
--- a/Documentation/Product Backlog.xlsx
+++ b/Documentation/Product Backlog.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\congv\Documents\Programming-Projects\COEN-390\Documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1F1E30-1CA9-4E64-A831-C0EB728BD370}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="5" r:id="rId1"/>
@@ -13,18 +19,15 @@
     <sheet name="Sprint 2" sheetId="3" r:id="rId4"/>
     <sheet name="Sprint 3" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="370">
   <si>
     <t>Story ID</t>
   </si>
@@ -316,22 +319,6 @@
     <t>Coding Arduino to send signals using Wfi.</t>
   </si>
   <si>
-    <t>Assigned to: Irfan Ahmed
-Priority 1</t>
-  </si>
-  <si>
-    <t>Assigned to: Irfan Ahmed
-Priority 5</t>
-  </si>
-  <si>
-    <t>Assigned to: Alec Kurkdjian
-Priority 1</t>
-  </si>
-  <si>
-    <t>Assigned to: Cong-Vinh Vu
-Priority 2</t>
-  </si>
-  <si>
     <t>Displays pictures taken by the camera in History page.</t>
   </si>
   <si>
@@ -380,9 +367,6 @@
     <t>Future</t>
   </si>
   <si>
-    <t>The camera takes picture of the person at the door and scans if it is an admin</t>
-  </si>
-  <si>
     <t>The gesture sensor opens the door for the user when used</t>
   </si>
   <si>
@@ -393,12 +377,6 @@
   </si>
   <si>
     <t>Completed</t>
-  </si>
-  <si>
-    <t>Coding Arduino to send camera pictures to Wifi server.</t>
-  </si>
-  <si>
-    <t>Testing</t>
   </si>
   <si>
     <t>Sprint 2</t>
@@ -432,9 +410,6 @@
     <t>• Confirmation from the stakeholders</t>
   </si>
   <si>
-    <t>Connect Arduino Database</t>
-  </si>
-  <si>
     <t>Camera Pictures to Database</t>
   </si>
   <si>
@@ -447,12 +422,6 @@
     <t>Add Lock</t>
   </si>
   <si>
-    <t>Arduino Holder</t>
-  </si>
-  <si>
-    <t>Sprint 3 Preparations</t>
-  </si>
-  <si>
     <t>Camera Holder</t>
   </si>
   <si>
@@ -510,9 +479,6 @@
     <t>Arduino and wifi module should be connected with good communication between both devices.</t>
   </si>
   <si>
-    <t>Arduino should be able to connect to the firebase server.</t>
-  </si>
-  <si>
     <t>The design of the app should be updated to the desired design.</t>
   </si>
   <si>
@@ -525,12 +491,6 @@
     <t>A 3D-printed model to be made to hold the camera.</t>
   </si>
   <si>
-    <t>A 3D-printed model to be made to hold the arduino by the door.</t>
-  </si>
-  <si>
-    <t>Documents needed for sprint 3 should be done.</t>
-  </si>
-  <si>
     <t>BE-2 &amp; BE-4</t>
   </si>
   <si>
@@ -540,12 +500,6 @@
     <t>BE-4.6</t>
   </si>
   <si>
-    <t>Arduino should be able to take instructions from Firebase and implement it.</t>
-  </si>
-  <si>
-    <t>Arduino should be able to send pictures to Firebase.</t>
-  </si>
-  <si>
     <t>The application should be able to send instructions to the database.</t>
   </si>
   <si>
@@ -576,10 +530,6 @@
     <t>WR</t>
   </si>
   <si>
-    <t>Assigned to: Cong-Vinh Vu
-Priority 1</t>
-  </si>
-  <si>
     <t>BE-6.2</t>
   </si>
   <si>
@@ -622,13 +572,6 @@
     <t>The application should not allow the usage of same emails and usernames.</t>
   </si>
   <si>
-    <t>Testing and validation of all task to be done in Sprint 2.</t>
-  </si>
-  <si>
-    <t>Assigned to: Cong-Vinh Vu &amp; Alec Kurkdjian
-Priority 3</t>
-  </si>
-  <si>
     <t>Delete Users</t>
   </si>
   <si>
@@ -638,21 +581,12 @@
     <t>As an administrator, I want the app to scan the picture of me it took at the door so that it verifies that I am an admin and unlock the door automatically for me. (Epic)</t>
   </si>
   <si>
-    <t>The user should be able to add additionnal doors to the appliaction, in order to access them by deleting other in Administrators page.</t>
-  </si>
-  <si>
     <t>Modify Profile</t>
   </si>
   <si>
-    <t>As an user, I want to be able remove others from the list of users to deny access to unwanted users. (Story)</t>
-  </si>
-  <si>
     <t>The user should be directed to a profile page to change her username, email, or password.</t>
   </si>
   <si>
-    <t>The applcaition should send an email to the user after clicking I Forgot My Password, to allow the user to reset their own password.</t>
-  </si>
-  <si>
     <t>As a user, I want to be able to create a profile so that I can myself as an administrator. (Story)</t>
   </si>
   <si>
@@ -698,19 +632,10 @@
     <t>• The history page shows the admin who opened the door along with the user that was at the door</t>
   </si>
   <si>
-    <t>• The pictures taken are scanned
-• The software distinguishes an admin from others
-• The only opens for admin after verification</t>
-  </si>
-  <si>
     <t>• The door opens with gestures</t>
   </si>
   <si>
     <t>• Clicking the button, opens the door</t>
-  </si>
-  <si>
-    <t>• The door is always locked
-• The door is locked after the door is closed</t>
   </si>
   <si>
     <t>• Display a list of all authorized users</t>
@@ -764,9 +689,6 @@
 • Credits button, when pressed, brings to the activity containing the collaborators information</t>
   </si>
   <si>
-    <t>Delete users by clicking a delete button in the Administrators page.</t>
-  </si>
-  <si>
     <t>Create a  profile page and allow user to modify their credentials.</t>
   </si>
   <si>
@@ -785,34 +707,6 @@
     <t>Ogo-Oluwa Jesutomi Olasubulumi: 40055693</t>
   </si>
   <si>
-    <t>Assigned to: Shadi Makdissi &amp; Ogo-Oluwa Jesutomi Olasubulumi
-Priority 1</t>
-  </si>
-  <si>
-    <t>Assigned to: Shadi Makdissi &amp; Ogo-Oluwa Jesutomi Olasubulumi
-Priority 2</t>
-  </si>
-  <si>
-    <t>Assigned to: Shadi Makdissi &amp; Ogo-Oluwa Jesutomi Olasubulumi
-Priority 3</t>
-  </si>
-  <si>
-    <t>Assigned to: Irfan Ahmed &amp; Alec Kurkdjian
-Priority 2</t>
-  </si>
-  <si>
-    <t>Assigned to: Irfan Ahmed
-Priority 3</t>
-  </si>
-  <si>
-    <t>Assigned to: Irfan Ahmed
-Priority 4</t>
-  </si>
-  <si>
-    <t>Assigned to: Shadi Makdissi &amp; Ogo-Oluwa Jesutomi Olasubulumi
-Priority 5</t>
-  </si>
-  <si>
     <t>Wifi Connected</t>
   </si>
   <si>
@@ -820,10 +714,6 @@
   </si>
   <si>
     <t>As a presenter, I want to know when the application is not connected to Wifi so that I can connect it manually. (Story)</t>
-  </si>
-  <si>
-    <t>Assigned to: Alec Kurkdjian &amp;  Irfan Ahmed
-Priority 2</t>
   </si>
   <si>
     <t>Sprint 1 Goal(s): Start the Applicationès Skeleton, Create Database, Coding and Testing of Sensors for Arduino</t>
@@ -916,9 +806,6 @@
     <t>BE-4.3</t>
   </si>
   <si>
-    <t>Sprint 2 Goal(s): Hardware Communication with Database and Finish Login Page, History Page, Administartors Page and, Start Peek Door</t>
-  </si>
-  <si>
     <t>RFID</t>
   </si>
   <si>
@@ -959,13 +846,365 @@
   </si>
   <si>
     <t>• Unlock the door using RFID</t>
+  </si>
+  <si>
+    <t>Priority 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Priority 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Priority 2</t>
+  </si>
+  <si>
+    <t>Priority 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Priority 3</t>
+  </si>
+  <si>
+    <t>Priority 4</t>
+  </si>
+  <si>
+    <t>Priority 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Priority 5</t>
+  </si>
+  <si>
+    <t>Rasberry-Pi should be able to take instructions from Firebase and implement it.</t>
+  </si>
+  <si>
+    <t>Rasberry-Pi should be able to connect to the firebase server.</t>
+  </si>
+  <si>
+    <t>Coding Rasberry-Pi to send camera pictures to Wifi server.</t>
+  </si>
+  <si>
+    <t>Rasberry-Pi  should be able to send pictures to Firebase.</t>
+  </si>
+  <si>
+    <t>Rasberry-Pi  Holder</t>
+  </si>
+  <si>
+    <t>A 3D-printed model to be made to hold the Rasberry-Pi  by the door.</t>
+  </si>
+  <si>
+    <t>Connect Rasberry-Pi Database</t>
+  </si>
+  <si>
+    <t>TEST-1</t>
+  </si>
+  <si>
+    <t>TEST-2</t>
+  </si>
+  <si>
+    <t>TEST-3</t>
+  </si>
+  <si>
+    <t>TEST-4</t>
+  </si>
+  <si>
+    <t>TEST-5</t>
+  </si>
+  <si>
+    <t>TEST-6</t>
+  </si>
+  <si>
+    <t>TEST-7</t>
+  </si>
+  <si>
+    <t>Testing Sign Up</t>
+  </si>
+  <si>
+    <t>Testing Login</t>
+  </si>
+  <si>
+    <t>Testing Peek Door</t>
+  </si>
+  <si>
+    <t>Testing Unlock Door</t>
+  </si>
+  <si>
+    <t>Testing History</t>
+  </si>
+  <si>
+    <t>Testing Administartors</t>
+  </si>
+  <si>
+    <t>Testing Edit Profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Piority 4</t>
+  </si>
+  <si>
+    <t>Unlocks the lock when card is near the sensor.</t>
+  </si>
+  <si>
+    <t>Testing and validation sign up page.</t>
+  </si>
+  <si>
+    <t>Testing and validation login page.</t>
+  </si>
+  <si>
+    <t>Testing and validation of peek door button and activty.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing and validation of unlock door </t>
+  </si>
+  <si>
+    <t>Testing and validation of history activity.</t>
+  </si>
+  <si>
+    <t>Testing and validation of administrators pages.</t>
+  </si>
+  <si>
+    <t>Testing and validation of edit profile feature.</t>
+  </si>
+  <si>
+    <t>Sprint 2 Goal(s): Hardware Communication with Database and Finish Login Page,  History Page,  Administartors Page,  Unlock Door and,  Peek Door</t>
+  </si>
+  <si>
+    <t>WR-1</t>
+  </si>
+  <si>
+    <t>WR-2</t>
+  </si>
+  <si>
+    <t>WR-3</t>
+  </si>
+  <si>
+    <t>WR-4</t>
+  </si>
+  <si>
+    <t>WR-5</t>
+  </si>
+  <si>
+    <t>Product Backlog and Sprint Grooming</t>
+  </si>
+  <si>
+    <t>Testing Documents</t>
+  </si>
+  <si>
+    <t>Definition of Done</t>
+  </si>
+  <si>
+    <t>Team Blog</t>
+  </si>
+  <si>
+    <t>Groming of Sprint 3 and Product Backlog. Update Sprint 2.</t>
+  </si>
+  <si>
+    <t>Follow the test plans and template.</t>
+  </si>
+  <si>
+    <t>Follow template on Moodle.</t>
+  </si>
+  <si>
+    <t>Follow template and discuss during team meetings.</t>
+  </si>
+  <si>
+    <t>GEN-13</t>
+  </si>
+  <si>
+    <t>GEN-14</t>
+  </si>
+  <si>
+    <t>GEN-15</t>
+  </si>
+  <si>
+    <t>GEN-16</t>
+  </si>
+  <si>
+    <t>Notification</t>
+  </si>
+  <si>
+    <t>GEN-17</t>
+  </si>
+  <si>
+    <t>Refactor Peek Door</t>
+  </si>
+  <si>
+    <t>Refactor Unlock Door</t>
+  </si>
+  <si>
+    <t>Refactor Edit Profile</t>
+  </si>
+  <si>
+    <t>Refactor History</t>
+  </si>
+  <si>
+    <t>As an administrator,  I want a responsive application to see who is at my door within seconds. (Story)</t>
+  </si>
+  <si>
+    <t>As an administrator,  I want a responsive application to unlock my door within seconds. (Story)</t>
+  </si>
+  <si>
+    <t>As an administrator,  I want a responsive application to update my profile within seconds. (Story)</t>
+  </si>
+  <si>
+    <t>As an administrator,  I want a responsive application to see the list of people who were at my door. (Story)</t>
+  </si>
+  <si>
+    <t>Peek Door should not sort all the images from a directory, rather use a given image url.</t>
+  </si>
+  <si>
+    <t>The code fro Rasberry-Pi should be clean and efficient.</t>
+  </si>
+  <si>
+    <t>• Peek Door should use the image url of its door
+• Peek Door should still function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+• Code should be clean and efficient
+• Unlock Door should still function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+• Code should be clean and efficient
+• Edit Profile should still function</t>
+  </si>
+  <si>
+    <t>Edit Proifle code shpuld be clean and readable. Any useless code should be removed and effcient solution should be found.</t>
+  </si>
+  <si>
+    <t>As an administrator, I want to get a notification when someone is at my door so that I can be readily available to open the door or deny access. (Story)</t>
+  </si>
+  <si>
+    <t>Send a notificatuon to the user when a new picture is taken and stored in the proper directory.</t>
+  </si>
+  <si>
+    <t>• Send a notifictaion when a new picture appears in the storage</t>
+  </si>
+  <si>
+    <t>On Hold</t>
+  </si>
+  <si>
+    <t>EX-3</t>
+  </si>
+  <si>
+    <t>EX-5</t>
+  </si>
+  <si>
+    <t>Multiple Doors</t>
+  </si>
+  <si>
+    <t>The database should allow the user to egister multiple doors per profile. Redo the datastructure of the profiles in the database. Unlock door shows a list of doors to unlock</t>
+  </si>
+  <si>
+    <t>As an administrator,  I to be able to access multiple doors per account so that I can manage my doors appropriately. (Epic)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+• Unlock doors show multiple doors to the user
+• Unlocks the appropriate door when button is clicked</t>
+  </si>
+  <si>
+    <t>The application should send an email to the user after clicking I Forgot My Password, to allow the user to reset their own password.</t>
+  </si>
+  <si>
+    <t>EX-6</t>
+  </si>
+  <si>
+    <t>Voice Recognition</t>
+  </si>
+  <si>
+    <t>As an user, I to be able to open my door using voice recognition to open the door with minimal actions. (Epic)</t>
+  </si>
+  <si>
+    <t>Use voice recognition to enable the door to open, store the voice of the user in the database.</t>
+  </si>
+  <si>
+    <t>Allows users to delete other unwanted usersusing a voting system.</t>
+  </si>
+  <si>
+    <t>• Deleted users should not be able to access the door
+• An user is only deleted if al of the mebers of that door vote him out other than himself</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+• If the voice of the user is registered to that door, open the door, else the door is locked</t>
+  </si>
+  <si>
+    <t>As an user, I want to be able remove others from the list of users to deny access to unwanted users. (story)</t>
+  </si>
+  <si>
+    <t>Priority 3</t>
+  </si>
+  <si>
+    <t>EX-2</t>
+  </si>
+  <si>
+    <t>The camera takes picture of the person at the door and scans if it is an administrator. Open the door if it is, else lock the door.</t>
+  </si>
+  <si>
+    <t>• The pictures taken are scanned
+• The software distinguishes an administrators from others
+• The only opens for administrators after verification</t>
+  </si>
+  <si>
+    <t>Final Report</t>
+  </si>
+  <si>
+    <t>Do final report.</t>
+  </si>
+  <si>
+    <t>WR-6</t>
+  </si>
+  <si>
+    <t>User Manual</t>
+  </si>
+  <si>
+    <t>Manual to show to the user how to use or application along side the hardware.</t>
+  </si>
+  <si>
+    <t>TEST-8</t>
+  </si>
+  <si>
+    <t>TEST-9</t>
+  </si>
+  <si>
+    <t>TEST-10</t>
+  </si>
+  <si>
+    <t>Testing Open Door</t>
+  </si>
+  <si>
+    <t>Testing AI</t>
+  </si>
+  <si>
+    <t>Testing and validation facial recognition feature.</t>
+  </si>
+  <si>
+    <t>Testing Reset Password</t>
+  </si>
+  <si>
+    <t>Testing and validation of reset password functionnality.</t>
+  </si>
+  <si>
+    <t>Sprint 3 Backlog</t>
+  </si>
+  <si>
+    <t>Sprint 3 Goal(s): Finish the entire application, add extra features such as facial recognition, have the physical door present,  and embellish our product</t>
+  </si>
+  <si>
+    <t>EX-2.1</t>
+  </si>
+  <si>
+    <t>We need to take many pictures and the AI needs to be trained to have an adequate success rate.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1437,89 +1676,89 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="126.7109375" customWidth="1"/>
+    <col min="1" max="1" width="126.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="7" customFormat="1" ht="13.5" customHeight="1"/>
-    <row r="2" spans="1:1" s="7" customFormat="1"/>
-    <row r="3" spans="1:1" s="7" customFormat="1" ht="26.25">
+    <row r="1" spans="1:1" s="7" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:1" s="7" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A3" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" s="7" customFormat="1"/>
-    <row r="5" spans="1:1" s="7" customFormat="1"/>
-    <row r="6" spans="1:1" s="7" customFormat="1" ht="21">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:1" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="7" customFormat="1">
+    <row r="7" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:1" s="7" customFormat="1" ht="21">
+    <row r="8" spans="1:1" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A8" s="9" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" s="7" customFormat="1"/>
-    <row r="10" spans="1:1" s="11" customFormat="1" ht="18.75">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:1" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" s="11" customFormat="1" ht="18.75">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" s="11" customFormat="1" ht="18.75">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" s="7" customFormat="1" ht="18.75">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" s="7" customFormat="1" ht="18.75">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" s="7" customFormat="1"/>
-    <row r="16" spans="1:1" s="7" customFormat="1"/>
-    <row r="17" s="7" customFormat="1"/>
-    <row r="18" s="7" customFormat="1"/>
-    <row r="19" s="7" customFormat="1"/>
-    <row r="20" s="7" customFormat="1"/>
-    <row r="21" s="7" customFormat="1"/>
-    <row r="22" s="7" customFormat="1"/>
-    <row r="23" s="7" customFormat="1"/>
-    <row r="24" s="7" customFormat="1"/>
-    <row r="25" s="7" customFormat="1"/>
-    <row r="26" s="7" customFormat="1"/>
-    <row r="27" s="7" customFormat="1"/>
-    <row r="28" s="7" customFormat="1"/>
-    <row r="29" s="7" customFormat="1"/>
-    <row r="30" s="7" customFormat="1"/>
+        <v>219</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="17" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="18" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="19" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="21" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="22" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="23" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="24" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="25" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="26" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="27" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="28" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="29" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="30" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -1527,30 +1766,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView topLeftCell="A43" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="16"/>
-    <col min="2" max="2" width="18.42578125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="44.42578125" style="16" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="16" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="16" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="46.7109375" style="16" customWidth="1"/>
-    <col min="8" max="8" width="42.5703125" style="16" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="16"/>
+    <col min="1" max="1" width="8.88671875" style="16"/>
+    <col min="2" max="2" width="18.44140625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="44.44140625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="16" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" style="16" customWidth="1"/>
+    <col min="7" max="7" width="46.6640625" style="16" customWidth="1"/>
+    <col min="8" max="8" width="42.5546875" style="16" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="24" t="s">
         <v>4</v>
       </c>
@@ -1562,7 +1801,7 @@
       <c r="G1" s="25"/>
       <c r="H1" s="25"/>
     </row>
-    <row r="5" spans="1:8" s="23" customFormat="1" ht="40.5" customHeight="1">
+    <row r="5" spans="1:8" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>0</v>
       </c>
@@ -1573,7 +1812,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>7</v>
@@ -1588,7 +1827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="120">
+    <row r="6" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>17</v>
       </c>
@@ -1605,16 +1844,16 @@
         <v>16</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G6" s="18" t="s">
         <v>50</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="20"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
@@ -1624,7 +1863,7 @@
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
     </row>
-    <row r="8" spans="1:8" ht="60">
+    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>20</v>
       </c>
@@ -1641,16 +1880,16 @@
         <v>16</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G8" s="18" t="s">
         <v>31</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="20"/>
       <c r="B9" s="15"/>
       <c r="C9" s="21"/>
@@ -1660,7 +1899,7 @@
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
     </row>
-    <row r="10" spans="1:8" ht="30">
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>25</v>
       </c>
@@ -1668,7 +1907,7 @@
         <v>42</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="D10" s="20">
         <v>3</v>
@@ -1677,16 +1916,16 @@
         <v>16</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G10" s="15" t="s">
         <v>44</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="20"/>
       <c r="B11" s="15"/>
       <c r="C11" s="21"/>
@@ -1696,7 +1935,7 @@
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
     </row>
-    <row r="12" spans="1:8" ht="45">
+    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>24</v>
       </c>
@@ -1704,7 +1943,7 @@
         <v>43</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="D12" s="20">
         <v>3</v>
@@ -1713,16 +1952,16 @@
         <v>16</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G12" s="15" t="s">
         <v>45</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="45">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>28</v>
       </c>
@@ -1730,7 +1969,7 @@
         <v>37</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="D13" s="20">
         <v>5</v>
@@ -1739,16 +1978,16 @@
         <v>16</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>53</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="20"/>
       <c r="B14" s="15"/>
       <c r="C14" s="21"/>
@@ -1758,7 +1997,7 @@
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
     </row>
-    <row r="15" spans="1:8" ht="45">
+    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>30</v>
       </c>
@@ -1766,7 +2005,7 @@
         <v>55</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D15" s="20">
         <v>3</v>
@@ -1775,16 +2014,16 @@
         <v>16</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G15" s="15" t="s">
         <v>56</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="20"/>
       <c r="B16" s="15"/>
       <c r="C16" s="21"/>
@@ -1794,7 +2033,7 @@
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
     </row>
-    <row r="17" spans="1:8" ht="45">
+    <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>29</v>
       </c>
@@ -1808,19 +2047,19 @@
         <v>3</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G17" s="15" t="s">
         <v>36</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="20"/>
       <c r="B18" s="15"/>
       <c r="C18" s="21"/>
@@ -1830,33 +2069,33 @@
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
     </row>
-    <row r="19" spans="1:8" ht="75">
+    <row r="19" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>251</v>
+        <v>220</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>253</v>
+        <v>222</v>
       </c>
       <c r="D19" s="20">
         <v>8</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>121</v>
+        <v>333</v>
       </c>
       <c r="G19" s="15" t="s">
         <v>85</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.6" customHeight="1">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="20"/>
       <c r="B20" s="15"/>
       <c r="C20" s="21"/>
@@ -1866,7 +2105,7 @@
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
     </row>
-    <row r="21" spans="1:8" ht="56.45" customHeight="1">
+    <row r="21" spans="1:8" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>41</v>
       </c>
@@ -1874,25 +2113,25 @@
         <v>71</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="D21" s="15">
         <v>5</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G21" s="15" t="s">
         <v>72</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="19.149999999999999" customHeight="1">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="20"/>
       <c r="B22" s="15"/>
       <c r="C22" s="21"/>
@@ -1902,7 +2141,7 @@
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
     </row>
-    <row r="23" spans="1:8" ht="61.9" customHeight="1">
+    <row r="23" spans="1:8" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>52</v>
       </c>
@@ -1910,26 +2149,26 @@
         <v>35</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D23" s="20">
         <v>5</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G23" s="15" t="s">
         <v>34</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="17.45" customHeight="1"/>
-    <row r="25" spans="1:8" ht="56.45" customHeight="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:8" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>22</v>
       </c>
@@ -1937,25 +2176,25 @@
         <v>38</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
       <c r="D25" s="20">
         <v>5</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G25" s="15" t="s">
         <v>33</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="20"/>
       <c r="B26" s="15"/>
       <c r="C26" s="21"/>
@@ -1965,33 +2204,33 @@
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
     </row>
-    <row r="27" spans="1:8" ht="56.45" customHeight="1">
+    <row r="27" spans="1:8" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
       <c r="D27" s="20">
         <v>2</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="20"/>
       <c r="B28" s="15"/>
       <c r="C28" s="21"/>
@@ -2001,33 +2240,33 @@
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
     </row>
-    <row r="29" spans="1:8" ht="60">
+    <row r="29" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
         <v>46</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
       <c r="D29" s="20">
         <v>3</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G29" s="15" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="H29" s="15" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="21" customHeight="1">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="20"/>
       <c r="B30" s="15"/>
       <c r="C30" s="21"/>
@@ -2037,33 +2276,33 @@
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>
     </row>
-    <row r="31" spans="1:8" ht="57" customHeight="1">
+    <row r="31" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="s">
-        <v>283</v>
+        <v>250</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>282</v>
+        <v>249</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>285</v>
+        <v>252</v>
       </c>
       <c r="D31" s="20">
         <v>3</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>286</v>
+        <v>253</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="20"/>
       <c r="B32" s="15"/>
       <c r="C32" s="21"/>
@@ -2073,33 +2312,33 @@
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
     </row>
-    <row r="33" spans="1:8" ht="60">
+    <row r="33" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
-        <v>284</v>
+        <v>251</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>277</v>
+        <v>244</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>288</v>
+        <v>255</v>
       </c>
       <c r="D33" s="20">
         <v>3</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>289</v>
+        <v>256</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="20"/>
       <c r="B34" s="15"/>
       <c r="C34" s="21"/>
@@ -2109,33 +2348,33 @@
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
     </row>
-    <row r="35" spans="1:8" ht="60">
+    <row r="35" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
       <c r="D35" s="20">
         <v>5</v>
       </c>
       <c r="E35" s="20" t="s">
-        <v>278</v>
+        <v>245</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>278</v>
+        <v>245</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="15.6" customHeight="1">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="20"/>
       <c r="B36" s="15"/>
       <c r="C36" s="21"/>
@@ -2145,33 +2384,33 @@
       <c r="G36" s="15"/>
       <c r="H36" s="15"/>
     </row>
-    <row r="37" spans="1:8" ht="61.9" customHeight="1">
+    <row r="37" spans="1:8" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="C37" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="D37" s="20">
+        <v>2</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="F37" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="G37" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="H37" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="D37" s="20">
-        <v>3</v>
-      </c>
-      <c r="E37" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="F37" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="G37" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="H37" s="15" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="15" customHeight="1">
+    </row>
+    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="20"/>
       <c r="B38" s="15"/>
       <c r="C38" s="21"/>
@@ -2181,33 +2420,33 @@
       <c r="G38" s="15"/>
       <c r="H38" s="15"/>
     </row>
-    <row r="39" spans="1:8" ht="45">
+    <row r="39" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="20" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
       <c r="D39" s="20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E39" s="20" t="s">
-        <v>278</v>
+        <v>245</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>278</v>
+        <v>245</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="17.45" customHeight="1">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="20"/>
       <c r="B40" s="15"/>
       <c r="C40" s="21"/>
@@ -2217,33 +2456,33 @@
       <c r="G40" s="15"/>
       <c r="H40" s="15"/>
     </row>
-    <row r="41" spans="1:8" ht="64.150000000000006" customHeight="1">
+    <row r="41" spans="1:8" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="D41" s="20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E41" s="20" t="s">
-        <v>278</v>
+        <v>245</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>278</v>
+        <v>245</v>
       </c>
       <c r="G41" s="15" t="s">
         <v>36</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="17.45" customHeight="1">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="20"/>
       <c r="B42" s="15"/>
       <c r="C42" s="21"/>
@@ -2253,33 +2492,33 @@
       <c r="G42" s="15"/>
       <c r="H42" s="15"/>
     </row>
-    <row r="43" spans="1:8" ht="45">
+    <row r="43" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="20" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>280</v>
+        <v>247</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="D43" s="20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E43" s="20" t="s">
-        <v>278</v>
+        <v>245</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>278</v>
+        <v>245</v>
       </c>
       <c r="G43" s="15" t="s">
         <v>36</v>
       </c>
       <c r="H43" s="15" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="20"/>
       <c r="B44" s="15"/>
       <c r="C44" s="21"/>
@@ -2289,33 +2528,33 @@
       <c r="G44" s="15"/>
       <c r="H44" s="15"/>
     </row>
-    <row r="45" spans="1:8" ht="45">
+    <row r="45" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" s="20" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="D45" s="20">
         <v>1</v>
       </c>
       <c r="E45" s="20" t="s">
-        <v>278</v>
+        <v>245</v>
       </c>
       <c r="F45" s="20" t="s">
-        <v>278</v>
+        <v>245</v>
       </c>
       <c r="G45" s="15" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="H45" s="15" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="20"/>
       <c r="B46" s="15"/>
       <c r="C46" s="21"/>
@@ -2325,33 +2564,33 @@
       <c r="G46" s="15"/>
       <c r="H46" s="15"/>
     </row>
-    <row r="47" spans="1:8" ht="45">
+    <row r="47" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A47" s="20" t="s">
-        <v>152</v>
+        <v>105</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>196</v>
+        <v>139</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="D47" s="20">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E47" s="20" t="s">
-        <v>278</v>
+        <v>245</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>278</v>
+        <v>245</v>
       </c>
       <c r="G47" s="15" t="s">
-        <v>199</v>
+        <v>351</v>
       </c>
       <c r="H47" s="15" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="20"/>
       <c r="B48" s="15"/>
       <c r="C48" s="21"/>
@@ -2361,33 +2600,33 @@
       <c r="G48" s="15"/>
       <c r="H48" s="15"/>
     </row>
-    <row r="49" spans="1:8" ht="60">
+    <row r="49" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="20" t="s">
-        <v>47</v>
+        <v>310</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>39</v>
+        <v>316</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>215</v>
+        <v>320</v>
       </c>
       <c r="D49" s="20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E49" s="20" t="s">
-        <v>113</v>
+        <v>245</v>
       </c>
       <c r="F49" s="20" t="s">
-        <v>110</v>
+        <v>245</v>
       </c>
       <c r="G49" s="15" t="s">
-        <v>32</v>
+        <v>324</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="20"/>
       <c r="B50" s="15"/>
       <c r="C50" s="21"/>
@@ -2397,33 +2636,33 @@
       <c r="G50" s="15"/>
       <c r="H50" s="15"/>
     </row>
-    <row r="51" spans="1:8" ht="60">
+    <row r="51" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" s="20" t="s">
-        <v>107</v>
+        <v>311</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>108</v>
+        <v>317</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>216</v>
+        <v>321</v>
       </c>
       <c r="D51" s="20">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E51" s="20" t="s">
-        <v>113</v>
+        <v>245</v>
       </c>
       <c r="F51" s="20" t="s">
-        <v>110</v>
+        <v>245</v>
       </c>
       <c r="G51" s="15" t="s">
-        <v>115</v>
+        <v>325</v>
       </c>
       <c r="H51" s="15" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="20"/>
       <c r="B52" s="15"/>
       <c r="C52" s="21"/>
@@ -2433,33 +2672,33 @@
       <c r="G52" s="15"/>
       <c r="H52" s="15"/>
     </row>
-    <row r="53" spans="1:8" ht="60">
+    <row r="53" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A53" s="20" t="s">
-        <v>109</v>
+        <v>315</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>149</v>
+        <v>318</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>198</v>
+        <v>322</v>
       </c>
       <c r="D53" s="20">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="E53" s="20" t="s">
-        <v>113</v>
+        <v>245</v>
       </c>
       <c r="F53" s="20" t="s">
-        <v>110</v>
+        <v>245</v>
       </c>
       <c r="G53" s="15" t="s">
-        <v>114</v>
+        <v>329</v>
       </c>
       <c r="H53" s="15" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="20"/>
       <c r="B54" s="15"/>
       <c r="C54" s="21"/>
@@ -2469,33 +2708,33 @@
       <c r="G54" s="15"/>
       <c r="H54" s="15"/>
     </row>
-    <row r="55" spans="1:8" ht="58.15" customHeight="1">
+    <row r="55" spans="1:8" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="20" t="s">
-        <v>117</v>
+        <v>313</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>148</v>
+        <v>314</v>
       </c>
       <c r="C55" s="21" t="s">
-        <v>217</v>
+        <v>330</v>
       </c>
       <c r="D55" s="20">
         <v>3</v>
       </c>
       <c r="E55" s="20" t="s">
-        <v>113</v>
+        <v>245</v>
       </c>
       <c r="F55" s="20" t="s">
-        <v>110</v>
+        <v>245</v>
       </c>
       <c r="G55" s="15" t="s">
-        <v>279</v>
+        <v>331</v>
       </c>
       <c r="H55" s="15" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="20"/>
       <c r="B56" s="15"/>
       <c r="C56" s="21"/>
@@ -2505,27 +2744,279 @@
       <c r="G56" s="15"/>
       <c r="H56" s="15"/>
     </row>
+    <row r="57" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A57" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C57" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="D57" s="20">
+        <v>3</v>
+      </c>
+      <c r="E57" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F57" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G57" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="H57" s="15" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" s="20"/>
+      <c r="B58" s="15"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="20"/>
+      <c r="E58" s="20"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="15"/>
+    </row>
+    <row r="59" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="B59" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C59" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="D59" s="20">
+        <v>13</v>
+      </c>
+      <c r="E59" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F59" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G59" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="H59" s="15" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" s="20"/>
+      <c r="B60" s="15"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="20"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="15"/>
+    </row>
+    <row r="61" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="B61" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C61" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="D61" s="20">
+        <v>3</v>
+      </c>
+      <c r="E61" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F61" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G61" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="H61" s="15" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" s="20"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="20"/>
+      <c r="E62" s="20"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15"/>
+    </row>
+    <row r="63" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A63" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B63" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="C63" s="21" t="s">
+        <v>323</v>
+      </c>
+      <c r="D63" s="20">
+        <v>5</v>
+      </c>
+      <c r="E63" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F63" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G63" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="H63" s="15" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64" s="20"/>
+      <c r="B64" s="15"/>
+      <c r="C64" s="21"/>
+      <c r="D64" s="20"/>
+      <c r="E64" s="20"/>
+      <c r="F64" s="20"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="15"/>
+    </row>
+    <row r="65" spans="1:8" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="B65" s="15" t="s">
+        <v>336</v>
+      </c>
+      <c r="C65" s="21" t="s">
+        <v>338</v>
+      </c>
+      <c r="D65" s="20">
+        <v>5</v>
+      </c>
+      <c r="E65" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F65" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G65" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="H65" s="15" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66" s="20"/>
+      <c r="B66" s="15"/>
+      <c r="C66" s="21"/>
+      <c r="D66" s="20"/>
+      <c r="E66" s="20"/>
+      <c r="F66" s="20"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15"/>
+    </row>
+    <row r="67" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="20" t="s">
+        <v>312</v>
+      </c>
+      <c r="B67" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="C67" s="21" t="s">
+        <v>348</v>
+      </c>
+      <c r="D67" s="20">
+        <v>3</v>
+      </c>
+      <c r="E67" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F67" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G67" s="15" t="s">
+        <v>345</v>
+      </c>
+      <c r="H67" s="15" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68" s="20"/>
+      <c r="B68" s="15"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="20"/>
+      <c r="E68" s="20"/>
+      <c r="F68" s="20"/>
+      <c r="G68" s="15"/>
+      <c r="H68" s="15"/>
+    </row>
+    <row r="69" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A69" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="B69" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="C69" s="21" t="s">
+        <v>343</v>
+      </c>
+      <c r="D69" s="20">
+        <v>13</v>
+      </c>
+      <c r="E69" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F69" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G69" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="H69" s="15" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70" s="20"/>
+      <c r="B70" s="15"/>
+      <c r="C70" s="21"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="20"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="15"/>
+      <c r="H70" s="15"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <dataValidations xWindow="650" yWindow="542" count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task status" prompt="Current status of task. One of: Planned, In Progress, On Hold, Completed" sqref="F57:F1048576 F4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task status" prompt="Current status of task. One of: Planned, In Progress, On Hold, Completed" sqref="F4 F68 F70 F73:F1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Planned, In Progress, On Hold, Completed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Priority" prompt="Priority of task. One of: Critical, High, Medium, Low" sqref="E57:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Priority" prompt="Priority of task. One of: Critical, High, Medium, Low" sqref="E68 E70 E73:E1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Critical, High, Medium, Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Story. One of: Planned, In Progress, On Hold, Completed" sqref="F6:F23 F25:F56">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Story. One of: Planned, In Progress, On Hold, Completed" sqref="F6:F23 F25:F70" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Not in sprint, Sprint 1, Sprint 2, Sprint 3, In Progress, On Hold, Completed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E6:E23 E25:E56">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E6:E23 E25:E70" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"Sprint 1, Sprint 2, Sprint 3, Future"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Is the task completed?" prompt="Describe the criteria to be used to determine if the task is completed as per requirements.&#10;" sqref="H5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Card. One of: Planned, In Progress, On Hold, Completed" sqref="F5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Story Point" prompt="Story point is an arbitary measure used to measure the effort required to implement a story.&#10;&#10;" sqref="D5"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Is the task completed?" prompt="Describe the criteria to be used to determine if the task is completed as per requirements._x000a_" sqref="H5" xr:uid="{00000000-0002-0000-0100-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Included in Sprint" prompt="Story included in which sprint. One of: Sprint 1, Sprint 2, Sprint 3, Future" sqref="E5" xr:uid="{00000000-0002-0000-0100-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Card Status" prompt="Current status of Card. One of: Planned, In Progress, On Hold, Completed" sqref="F5" xr:uid="{00000000-0002-0000-0100-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Story Point" prompt="Story point is an arbitary measure used to measure the effort required to implement a story._x000a__x000a_" sqref="D5" xr:uid="{00000000-0002-0000-0100-000007000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="60" orientation="landscape" r:id="rId1"/>
@@ -2533,26 +3024,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="25.140625" customWidth="1"/>
-    <col min="4" max="4" width="44.42578125" customWidth="1"/>
-    <col min="5" max="6" width="7.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="43.140625" customWidth="1"/>
+    <col min="3" max="3" width="25.109375" customWidth="1"/>
+    <col min="4" max="4" width="44.44140625" customWidth="1"/>
+    <col min="5" max="6" width="7.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" customWidth="1"/>
+    <col min="8" max="8" width="43.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>5</v>
       </c>
@@ -2564,9 +3055,9 @@
       <c r="G1" s="26"/>
       <c r="H1" s="26"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
-        <v>255</v>
+        <v>223</v>
       </c>
       <c r="B4" s="27"/>
       <c r="C4" s="27"/>
@@ -2575,7 +3066,7 @@
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="28" t="s">
         <v>81</v>
       </c>
@@ -2585,7 +3076,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="6" customFormat="1" ht="40.5" customHeight="1">
+    <row r="6" spans="1:8" s="6" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
@@ -2609,7 +3100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="135">
+    <row r="7" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -2629,13 +3120,13 @@
         <v>78</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="60">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -2655,24 +3146,24 @@
         <v>78</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="60">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E9" s="3">
         <v>5</v>
@@ -2681,13 +3172,13 @@
         <v>78</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="60">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -2698,7 +3189,7 @@
         <v>42</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E10" s="3">
         <v>3</v>
@@ -2707,13 +3198,13 @@
         <v>78</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="60">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
@@ -2724,7 +3215,7 @@
         <v>43</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E11" s="3">
         <v>5</v>
@@ -2733,13 +3224,13 @@
         <v>78</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="75">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
@@ -2759,13 +3250,13 @@
         <v>78</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="45">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>30</v>
       </c>
@@ -2785,13 +3276,13 @@
         <v>78</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="60">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
@@ -2811,13 +3302,13 @@
         <v>78</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="75">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>30</v>
       </c>
@@ -2837,13 +3328,13 @@
         <v>78</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="45">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
@@ -2863,13 +3354,13 @@
         <v>78</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="60">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
@@ -2889,13 +3380,13 @@
         <v>78</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="45">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>29</v>
       </c>
@@ -2915,13 +3406,13 @@
         <v>78</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="45">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>29</v>
       </c>
@@ -2941,13 +3432,13 @@
         <v>78</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="45">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>29</v>
       </c>
@@ -2967,13 +3458,13 @@
         <v>78</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="45">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>41</v>
       </c>
@@ -2993,13 +3484,13 @@
         <v>78</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="60">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>41</v>
       </c>
@@ -3019,24 +3510,24 @@
         <v>78</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="30">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>275</v>
+        <v>243</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>272</v>
+        <v>240</v>
       </c>
       <c r="E23" s="2">
         <v>5</v>
@@ -3045,24 +3536,24 @@
         <v>78</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="45">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E24" s="2">
         <v>5</v>
@@ -3071,10 +3562,10 @@
         <v>78</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>274</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -3084,9 +3575,9 @@
     <mergeCell ref="A5:B5"/>
   </mergeCells>
   <dataValidations xWindow="1022" yWindow="574" count="3">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G6"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimate" prompt="Estimated hours for the task." sqref="E6:F6"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G7:G20 G21:G24">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G6" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimate" prompt="Estimated hours for the task." sqref="E6:F6" xr:uid="{00000000-0002-0000-0200-000001000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G7:G20 G21:G24" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>"Planned, In Progress, On Hold, Completed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3096,26 +3587,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" customWidth="1"/>
+    <col min="4" max="4" width="25.44140625" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -3125,9 +3616,9 @@
       <c r="G1" s="26"/>
       <c r="H1" s="26"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="B4" s="29"/>
       <c r="C4" s="29"/>
@@ -3137,17 +3628,17 @@
       <c r="G4" s="29"/>
       <c r="H4" s="29"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="28" t="s">
         <v>81</v>
       </c>
       <c r="B5" s="28"/>
       <c r="C5">
-        <f>SUM(E3:E31)</f>
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="30">
+        <f>SUM(E3:E30)</f>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
@@ -3171,18 +3662,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="60">
+    <row r="7" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>281</v>
+        <v>248</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="E7" s="3">
         <v>5</v>
@@ -3191,13 +3682,13 @@
         <v>78</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>15</v>
+        <v>113</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="60">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>48</v>
       </c>
@@ -3217,24 +3708,24 @@
         <v>78</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>15</v>
+        <v>113</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="30">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>43</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="E9" s="2">
         <v>2</v>
@@ -3243,24 +3734,24 @@
         <v>78</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>15</v>
+        <v>113</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="45">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>43</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="E10" s="2">
         <v>3</v>
@@ -3269,24 +3760,24 @@
         <v>78</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>15</v>
+        <v>113</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="45">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>43</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="E11" s="2">
         <v>3</v>
@@ -3295,24 +3786,24 @@
         <v>78</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>15</v>
+        <v>113</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="30">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="E12" s="2">
         <v>2</v>
@@ -3321,24 +3812,24 @@
         <v>78</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>15</v>
+        <v>113</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="60">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>37</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="E13" s="2">
         <v>3</v>
@@ -3347,128 +3838,128 @@
         <v>78</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>15</v>
+        <v>113</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="30">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>160</v>
+        <v>144</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>145</v>
       </c>
       <c r="E14" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>15</v>
+      <c r="G14" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="60">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="C15" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="E15" s="2">
+        <v>4</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="E16" s="3">
+        <v>5</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D17" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="D15" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="E15" s="2">
-        <v>5</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="45">
-      <c r="A16" s="2" t="s">
+      <c r="E17" s="2">
+        <v>3</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>237</v>
-      </c>
-      <c r="E16" s="2">
-        <v>4</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="45">
-      <c r="A17" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>238</v>
-      </c>
-      <c r="E17" s="2">
-        <v>4</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="60">
-      <c r="A18" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>172</v>
-      </c>
       <c r="C18" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>167</v>
+        <v>272</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>267</v>
       </c>
       <c r="E18" s="3">
         <v>5</v>
@@ -3477,347 +3968,401 @@
         <v>78</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>15</v>
+        <v>113</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="45">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>142</v>
+        <v>27</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>176</v>
+        <v>27</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>170</v>
+        <v>220</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>169</v>
+        <v>221</v>
       </c>
       <c r="E19" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G19" s="3" t="s">
-        <v>15</v>
+      <c r="G19" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="60">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="E20" s="3">
+        <v>41</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="E20" s="2">
         <v>5</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>15</v>
+      <c r="F20" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="60">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="E21" s="3">
+        <v>5</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="D21" s="13" t="s">
-        <v>252</v>
-      </c>
-      <c r="E21" s="2">
-        <v>5</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H21" s="13" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="87" customHeight="1">
-      <c r="A22" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="E22" s="2">
-        <v>5</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>15</v>
+      <c r="B22" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="E22" s="3">
+        <v>4</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="60">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>123</v>
+        <v>162</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>180</v>
+        <v>273</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>122</v>
+        <v>280</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>182</v>
+        <v>289</v>
       </c>
       <c r="E23" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>15</v>
+      <c r="G23" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="30.75" customHeight="1">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>41</v>
+        <v>162</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>105</v>
+        <v>274</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>91</v>
+        <v>281</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>119</v>
+        <v>290</v>
       </c>
       <c r="E24" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>15</v>
+      <c r="G24" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="45" customHeight="1">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="E25" s="3">
-        <v>5</v>
-      </c>
-      <c r="F25" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>78</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>15</v>
+        <v>113</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="45">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>127</v>
+        <v>162</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>127</v>
+        <v>276</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>128</v>
+        <v>283</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>158</v>
+        <v>292</v>
       </c>
       <c r="E26" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>78</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>15</v>
+        <v>113</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="45">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>175</v>
+        <v>277</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>134</v>
+        <v>284</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>159</v>
+        <v>293</v>
       </c>
       <c r="E27" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>78</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>15</v>
+        <v>113</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="30">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>151</v>
+        <v>278</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>138</v>
+        <v>285</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>161</v>
+        <v>294</v>
       </c>
       <c r="E28" s="2">
+        <v>1</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="E29" s="2">
+        <v>1</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="E30" s="2">
         <v>2</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H28" s="13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="60">
-      <c r="A29" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="E29" s="2">
-        <v>4</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H29" s="13" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="45">
-      <c r="A30" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="E30" s="2">
-        <v>4</v>
-      </c>
       <c r="F30" s="2" t="s">
         <v>78</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>15</v>
+        <v>113</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="30">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>178</v>
+        <v>298</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>137</v>
+        <v>303</v>
       </c>
       <c r="D31" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="E31" s="2">
+        <v>2</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="E31" s="2">
-        <v>3</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H31" s="13"/>
+      <c r="B32" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="E32" s="2">
+        <v>2</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="E33" s="2">
+        <v>2</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>264</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3826,11 +4371,11 @@
     <mergeCell ref="A4:H4"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G7:G31">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimate" prompt="Estimated hours for the task." sqref="E6:F6" xr:uid="{00000000-0002-0000-0300-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G6" xr:uid="{00000000-0002-0000-0300-000002000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G7:G33" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Planned, In Progress, On Hold, Completed"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimate" prompt="Estimated hours for the task." sqref="E6:F6"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G6"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3838,13 +4383,856 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+    </row>
+    <row r="3" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="29" t="s">
+        <v>367</v>
+      </c>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="28"/>
+      <c r="C5">
+        <f>SUM(E3:E33)</f>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="E8" s="2">
+        <v>5</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>340</v>
+      </c>
+      <c r="E9" s="2">
+        <v>5</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="E11" s="2">
+        <v>5</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E12" s="2">
+        <v>5</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="E13" s="2">
+        <v>5</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>329</v>
+      </c>
+      <c r="E14" s="2">
+        <v>3</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="E15" s="2">
+        <v>2</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="E17" s="2">
+        <v>3</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>369</v>
+      </c>
+      <c r="E18" s="2">
+        <v>5</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="E19" s="2">
+        <v>5</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="E26" s="2">
+        <v>1</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>362</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>365</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="E29" s="2">
+        <v>1</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="E30" s="2">
+        <v>2</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="E31" s="2">
+        <v>2</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="E32" s="2">
+        <v>2</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="E33" s="2">
+        <v>2</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="E34" s="2">
+        <v>4</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>357</v>
+      </c>
+      <c r="E35" s="2">
+        <v>3</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>264</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A3:H4"/>
+  </mergeCells>
+  <dataValidations count="3">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G6" xr:uid="{34C57A29-108F-4915-BF51-E2DB1CB55948}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estimate" prompt="Estimated hours for the task." sqref="E6:F6" xr:uid="{7B4CB452-2384-49D7-A90B-85376000E5F1}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Status" prompt="Current status of Task. One of: Planned, In Progress, On Hold, Completed" sqref="G7:G35" xr:uid="{00000000-0002-0000-0300-000000000000}">
+      <formula1>"Planned, In Progress, On Hold, Completed"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
updated backlog and Team Blog
</commit_message>
<xml_diff>
--- a/Documentation/Product Backlog.xlsx
+++ b/Documentation/Product Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomil\StudioProjects\ELEC-COEN-390\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1105D28-28C0-4407-A2CC-A9F5E3942946}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B270F228-A873-4314-AC65-043FA7B881E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="5" r:id="rId1"/>
@@ -808,9 +808,6 @@
     <t>Rasberry -Pi Holder</t>
   </si>
   <si>
-    <t>Connect Rasberry -Pi Wifi</t>
-  </si>
-  <si>
     <t>Refactor Display History</t>
   </si>
   <si>
@@ -1346,6 +1343,9 @@
   </si>
   <si>
     <t>Monitor Admin's Entry</t>
+  </si>
+  <si>
+    <t>Connectionof Rasberry -Pi Wifi</t>
   </si>
 </sst>
 </file>
@@ -1920,8 +1920,8 @@
   </sheetPr>
   <dimension ref="A1:H88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2405,7 +2405,7 @@
         <v>46</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C29" s="21" t="s">
         <v>185</v>
@@ -2420,7 +2420,7 @@
         <v>113</v>
       </c>
       <c r="G29" s="15" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="H29" s="15" t="s">
         <v>198</v>
@@ -2438,13 +2438,13 @@
     </row>
     <row r="31" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D31" s="20">
         <v>3</v>
@@ -2456,10 +2456,10 @@
         <v>113</v>
       </c>
       <c r="G31" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="H31" s="15" t="s">
         <v>249</v>
-      </c>
-      <c r="H31" s="15" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -2474,13 +2474,13 @@
     </row>
     <row r="33" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B33" s="15" t="s">
         <v>240</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D33" s="20">
         <v>3</v>
@@ -2492,10 +2492,10 @@
         <v>113</v>
       </c>
       <c r="G33" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="H33" s="15" t="s">
         <v>252</v>
-      </c>
-      <c r="H33" s="15" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -2744,10 +2744,10 @@
         <v>113</v>
       </c>
       <c r="G47" s="15" t="s">
+        <v>343</v>
+      </c>
+      <c r="H47" s="15" t="s">
         <v>344</v>
-      </c>
-      <c r="H47" s="15" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
@@ -2762,13 +2762,13 @@
     </row>
     <row r="49" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="20" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D49" s="20">
         <v>2</v>
@@ -2780,10 +2780,10 @@
         <v>113</v>
       </c>
       <c r="G49" s="15" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
@@ -2798,13 +2798,13 @@
     </row>
     <row r="51" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" s="20" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D51" s="20">
         <v>2</v>
@@ -2816,10 +2816,10 @@
         <v>113</v>
       </c>
       <c r="G51" s="15" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H51" s="15" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
@@ -2834,13 +2834,13 @@
     </row>
     <row r="53" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A53" s="20" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D53" s="20">
         <v>2</v>
@@ -2852,10 +2852,10 @@
         <v>113</v>
       </c>
       <c r="G53" s="15" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H53" s="15" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
@@ -2870,13 +2870,13 @@
     </row>
     <row r="55" spans="1:8" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="20" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C55" s="21" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D55" s="20">
         <v>3</v>
@@ -2888,10 +2888,10 @@
         <v>113</v>
       </c>
       <c r="G55" s="15" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H55" s="15" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
@@ -2978,10 +2978,10 @@
     </row>
     <row r="61" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A61" s="20" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C61" s="21" t="s">
         <v>192</v>
@@ -3017,10 +3017,10 @@
         <v>112</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C63" s="21" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D63" s="20">
         <v>5</v>
@@ -3050,13 +3050,13 @@
     </row>
     <row r="65" spans="1:8" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="20" t="s">
+        <v>328</v>
+      </c>
+      <c r="B65" s="15" t="s">
         <v>329</v>
       </c>
-      <c r="B65" s="15" t="s">
-        <v>330</v>
-      </c>
       <c r="C65" s="21" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D65" s="20">
         <v>5</v>
@@ -3068,10 +3068,10 @@
         <v>106</v>
       </c>
       <c r="G65" s="15" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H65" s="15" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
@@ -3086,13 +3086,13 @@
     </row>
     <row r="67" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A67" s="20" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B67" s="15" t="s">
         <v>174</v>
       </c>
       <c r="C67" s="21" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D67" s="20">
         <v>3</v>
@@ -3104,10 +3104,10 @@
         <v>106</v>
       </c>
       <c r="G67" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="H67" s="15" t="s">
         <v>338</v>
-      </c>
-      <c r="H67" s="15" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
@@ -3122,13 +3122,13 @@
     </row>
     <row r="69" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A69" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="B69" s="15" t="s">
         <v>335</v>
       </c>
-      <c r="B69" s="15" t="s">
-        <v>336</v>
-      </c>
       <c r="C69" s="21" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D69" s="20">
         <v>13</v>
@@ -3140,10 +3140,10 @@
         <v>106</v>
       </c>
       <c r="G69" s="15" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H69" s="15" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
@@ -3158,13 +3158,13 @@
     </row>
     <row r="71" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A71" s="20" t="s">
+        <v>364</v>
+      </c>
+      <c r="B71" s="15" t="s">
         <v>365</v>
       </c>
-      <c r="B71" s="15" t="s">
-        <v>366</v>
-      </c>
       <c r="C71" s="21" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D71" s="20">
         <v>13</v>
@@ -3176,10 +3176,10 @@
         <v>106</v>
       </c>
       <c r="G71" s="15" t="s">
+        <v>368</v>
+      </c>
+      <c r="H71" s="15" t="s">
         <v>369</v>
-      </c>
-      <c r="H71" s="15" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
@@ -3194,13 +3194,13 @@
     </row>
     <row r="73" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A73" s="20" t="s">
+        <v>372</v>
+      </c>
+      <c r="B73" s="15" t="s">
         <v>373</v>
       </c>
-      <c r="B73" s="15" t="s">
-        <v>374</v>
-      </c>
       <c r="C73" s="21" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D73" s="20">
         <v>8</v>
@@ -3212,10 +3212,10 @@
         <v>106</v>
       </c>
       <c r="G73" s="15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H73" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
@@ -3230,13 +3230,13 @@
     </row>
     <row r="75" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A75" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="B75" s="15" t="s">
         <v>375</v>
       </c>
-      <c r="B75" s="15" t="s">
-        <v>376</v>
-      </c>
       <c r="C75" s="21" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D75" s="20">
         <v>8</v>
@@ -3248,10 +3248,10 @@
         <v>106</v>
       </c>
       <c r="G75" s="15" t="s">
+        <v>383</v>
+      </c>
+      <c r="H75" s="15" t="s">
         <v>384</v>
-      </c>
-      <c r="H75" s="15" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
@@ -3266,13 +3266,13 @@
     </row>
     <row r="77" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A77" s="20" t="s">
+        <v>376</v>
+      </c>
+      <c r="B77" s="15" t="s">
         <v>377</v>
       </c>
-      <c r="B77" s="15" t="s">
-        <v>378</v>
-      </c>
       <c r="C77" s="21" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D77" s="20">
         <v>5</v>
@@ -3284,10 +3284,10 @@
         <v>106</v>
       </c>
       <c r="G77" s="15" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H77" s="15" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
@@ -3302,13 +3302,13 @@
     </row>
     <row r="79" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A79" s="20" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B79" s="15" t="s">
+        <v>405</v>
+      </c>
+      <c r="C79" s="21" t="s">
         <v>406</v>
-      </c>
-      <c r="C79" s="21" t="s">
-        <v>407</v>
       </c>
       <c r="D79" s="20">
         <v>13</v>
@@ -3320,10 +3320,10 @@
         <v>106</v>
       </c>
       <c r="G79" s="15" t="s">
+        <v>407</v>
+      </c>
+      <c r="H79" s="15" t="s">
         <v>408</v>
-      </c>
-      <c r="H79" s="15" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
@@ -3338,13 +3338,13 @@
     </row>
     <row r="81" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A81" s="20" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B81" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C81" s="21" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D81" s="20">
         <v>1</v>
@@ -3356,10 +3356,10 @@
         <v>106</v>
       </c>
       <c r="G81" s="15" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H81" s="15" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
@@ -3374,13 +3374,13 @@
     </row>
     <row r="83" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A83" s="20" t="s">
+        <v>390</v>
+      </c>
+      <c r="B83" s="15" t="s">
         <v>391</v>
       </c>
-      <c r="B83" s="15" t="s">
-        <v>392</v>
-      </c>
       <c r="C83" s="21" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D83" s="20">
         <v>3</v>
@@ -3392,10 +3392,10 @@
         <v>106</v>
       </c>
       <c r="G83" s="15" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H83" s="15" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
@@ -3410,13 +3410,13 @@
     </row>
     <row r="85" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A85" s="20" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B85" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="C85" s="21" t="s">
         <v>395</v>
-      </c>
-      <c r="C85" s="21" t="s">
-        <v>396</v>
       </c>
       <c r="D85" s="20">
         <v>2</v>
@@ -3428,10 +3428,10 @@
         <v>106</v>
       </c>
       <c r="G85" s="15" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="H85" s="15" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
@@ -3446,13 +3446,13 @@
     </row>
     <row r="87" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A87" s="20" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B87" s="15" t="s">
+        <v>409</v>
+      </c>
+      <c r="C87" s="21" t="s">
         <v>410</v>
-      </c>
-      <c r="C87" s="21" t="s">
-        <v>411</v>
       </c>
       <c r="D87" s="20">
         <v>3</v>
@@ -3464,10 +3464,10 @@
         <v>106</v>
       </c>
       <c r="G87" s="15" t="s">
+        <v>411</v>
+      </c>
+      <c r="H87" s="15" t="s">
         <v>412</v>
-      </c>
-      <c r="H87" s="15" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
@@ -3515,8 +3515,8 @@
   </sheetPr>
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4075,8 +4075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4103,7 +4103,7 @@
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B4" s="29"/>
       <c r="C4" s="29"/>
@@ -4155,10 +4155,10 @@
         <v>150</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>244</v>
+        <v>415</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E7" s="3">
         <v>2</v>
@@ -4170,7 +4170,7 @@
         <v>113</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -4196,7 +4196,7 @@
         <v>113</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4222,7 +4222,7 @@
         <v>113</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -4248,7 +4248,7 @@
         <v>113</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -4274,7 +4274,7 @@
         <v>113</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4300,7 +4300,7 @@
         <v>113</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -4326,7 +4326,7 @@
         <v>113</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4352,7 +4352,7 @@
         <v>113</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -4363,10 +4363,10 @@
         <v>46</v>
       </c>
       <c r="C15" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="D15" s="14" t="s">
         <v>371</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>372</v>
       </c>
       <c r="E15" s="2">
         <v>3</v>
@@ -4378,7 +4378,7 @@
         <v>113</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -4404,7 +4404,7 @@
         <v>113</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -4430,7 +4430,7 @@
         <v>113</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -4444,7 +4444,7 @@
         <v>125</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E18" s="3">
         <v>5</v>
@@ -4456,7 +4456,7 @@
         <v>113</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -4482,7 +4482,7 @@
         <v>113</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -4493,10 +4493,10 @@
         <v>150</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E20" s="3">
         <v>5</v>
@@ -4508,7 +4508,7 @@
         <v>113</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -4534,7 +4534,7 @@
         <v>113</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4548,7 +4548,7 @@
         <v>91</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E22" s="2">
         <v>5</v>
@@ -4560,7 +4560,7 @@
         <v>113</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4574,7 +4574,7 @@
         <v>124</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E23" s="3">
         <v>5</v>
@@ -4586,21 +4586,21 @@
         <v>113</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>240</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E24" s="3">
         <v>4</v>
@@ -4612,7 +4612,7 @@
         <v>113</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -4620,13 +4620,13 @@
         <v>158</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E25" s="2">
         <v>1</v>
@@ -4638,7 +4638,7 @@
         <v>113</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4646,13 +4646,13 @@
         <v>158</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E26" s="2">
         <v>1</v>
@@ -4664,7 +4664,7 @@
         <v>113</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4672,13 +4672,13 @@
         <v>158</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E27" s="2">
         <v>1</v>
@@ -4690,7 +4690,7 @@
         <v>113</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4698,13 +4698,13 @@
         <v>158</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E28" s="2">
         <v>1</v>
@@ -4716,7 +4716,7 @@
         <v>113</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4724,13 +4724,13 @@
         <v>158</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E29" s="2">
         <v>1</v>
@@ -4742,7 +4742,7 @@
         <v>113</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4750,13 +4750,13 @@
         <v>158</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E30" s="2">
         <v>1</v>
@@ -4768,7 +4768,7 @@
         <v>113</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4776,13 +4776,13 @@
         <v>158</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E31" s="2">
         <v>1</v>
@@ -4794,7 +4794,7 @@
         <v>113</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -4802,13 +4802,13 @@
         <v>159</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E32" s="2">
         <v>2</v>
@@ -4820,7 +4820,7 @@
         <v>113</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4828,13 +4828,13 @@
         <v>159</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E33" s="2">
         <v>2</v>
@@ -4846,7 +4846,7 @@
         <v>113</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -4854,13 +4854,13 @@
         <v>159</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E34" s="2">
         <v>2</v>
@@ -4872,7 +4872,7 @@
         <v>113</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4880,13 +4880,13 @@
         <v>159</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E35" s="2">
         <v>2</v>
@@ -4898,7 +4898,7 @@
         <v>113</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -4923,7 +4923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -4937,7 +4937,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -4949,7 +4949,7 @@
     </row>
     <row r="3" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B3" s="29"/>
       <c r="C3" s="29"/>
@@ -5026,21 +5026,21 @@
         <v>15</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C8" s="13" t="s">
         <v>309</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>310</v>
-      </c>
       <c r="D8" s="13" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E8" s="2">
         <v>5</v>
@@ -5052,7 +5052,7 @@
         <v>15</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
@@ -5066,7 +5066,7 @@
         <v>115</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E9" s="2">
         <v>5</v>
@@ -5078,7 +5078,7 @@
         <v>15</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -5104,21 +5104,21 @@
         <v>15</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E11" s="2">
         <v>5</v>
@@ -5130,7 +5130,7 @@
         <v>15</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5156,21 +5156,21 @@
         <v>15</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E13" s="2">
         <v>5</v>
@@ -5182,21 +5182,21 @@
         <v>15</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E14" s="2">
         <v>3</v>
@@ -5208,7 +5208,7 @@
         <v>15</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5234,7 +5234,7 @@
         <v>15</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -5245,10 +5245,10 @@
         <v>141</v>
       </c>
       <c r="C16" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="D16" s="13" t="s">
         <v>266</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>267</v>
       </c>
       <c r="E16" s="2">
         <v>2</v>
@@ -5260,7 +5260,7 @@
         <v>15</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -5286,21 +5286,21 @@
         <v>15</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>138</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E18" s="2">
         <v>5</v>
@@ -5312,21 +5312,21 @@
         <v>15</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>138</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E19" s="2">
         <v>5</v>
@@ -5338,7 +5338,7 @@
         <v>15</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5346,13 +5346,13 @@
         <v>158</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E20" s="2">
         <v>1</v>
@@ -5364,7 +5364,7 @@
         <v>15</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5372,13 +5372,13 @@
         <v>158</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E21" s="2">
         <v>1</v>
@@ -5390,7 +5390,7 @@
         <v>15</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5398,13 +5398,13 @@
         <v>158</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E22" s="2">
         <v>1</v>
@@ -5416,7 +5416,7 @@
         <v>15</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5424,13 +5424,13 @@
         <v>158</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E23" s="2">
         <v>1</v>
@@ -5442,7 +5442,7 @@
         <v>15</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5450,13 +5450,13 @@
         <v>158</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E24" s="2">
         <v>1</v>
@@ -5468,7 +5468,7 @@
         <v>15</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5476,13 +5476,13 @@
         <v>158</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E25" s="2">
         <v>1</v>
@@ -5494,7 +5494,7 @@
         <v>15</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5502,13 +5502,13 @@
         <v>158</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E26" s="2">
         <v>1</v>
@@ -5520,7 +5520,7 @@
         <v>15</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5528,13 +5528,13 @@
         <v>158</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C27" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="D27" s="13" t="s">
         <v>355</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>356</v>
       </c>
       <c r="E27" s="2">
         <v>2</v>
@@ -5546,7 +5546,7 @@
         <v>15</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5554,13 +5554,13 @@
         <v>158</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C28" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="D28" s="13" t="s">
         <v>357</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>358</v>
       </c>
       <c r="E28" s="2">
         <v>1</v>
@@ -5572,7 +5572,7 @@
         <v>15</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5580,13 +5580,13 @@
         <v>158</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C29" s="13" t="s">
         <v>353</v>
       </c>
-      <c r="C29" s="13" t="s">
-        <v>354</v>
-      </c>
       <c r="D29" s="13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E29" s="2">
         <v>1</v>
@@ -5598,7 +5598,7 @@
         <v>15</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -5606,13 +5606,13 @@
         <v>159</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E30" s="2">
         <v>2</v>
@@ -5624,7 +5624,7 @@
         <v>15</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5632,13 +5632,13 @@
         <v>159</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E31" s="2">
         <v>2</v>
@@ -5650,7 +5650,7 @@
         <v>15</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5658,13 +5658,13 @@
         <v>159</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E32" s="2">
         <v>2</v>
@@ -5676,7 +5676,7 @@
         <v>15</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5684,13 +5684,13 @@
         <v>159</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E33" s="2">
         <v>2</v>
@@ -5702,7 +5702,7 @@
         <v>15</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -5710,13 +5710,13 @@
         <v>159</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C34" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="D34" s="13" t="s">
         <v>346</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>347</v>
       </c>
       <c r="E34" s="2">
         <v>4</v>
@@ -5728,7 +5728,7 @@
         <v>15</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -5736,13 +5736,13 @@
         <v>159</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C35" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="D35" s="13" t="s">
         <v>349</v>
-      </c>
-      <c r="D35" s="13" t="s">
-        <v>350</v>
       </c>
       <c r="E35" s="2">
         <v>3</v>
@@ -5754,7 +5754,7 @@
         <v>15</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>